<commit_message>
fully implemented masks and filters for devices, update specifications
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89280EA-FA51-4982-AE68-96EC625F1D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83367951-A0CB-4C44-AEA0-5E81D5FB8FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
+    <workbookView xWindow="3255" yWindow="735" windowWidth="21585" windowHeight="11340" activeTab="2" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
   <sheets>
     <sheet name="frames-data-bits" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="273">
   <si>
     <t>temperature</t>
   </si>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABEE202-717B-4A96-9406-D9A14283F0F2}">
   <dimension ref="B1:AH50"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4818,7 +4818,7 @@
   <dimension ref="A2:BO45"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9012,8 +9012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36880ADF-04C9-4A12-8EFC-224812D037A0}">
   <dimension ref="A3:K87"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10813,20 +10813,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BCC11E-390E-4EFB-A4DD-B5D6139D8CF5}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="D10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="4" max="14" width="3.42578125" style="67" customWidth="1"/>
+    <col min="15" max="35" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B2" s="226" t="s">
         <v>232</v>
       </c>
@@ -10845,9 +10846,28 @@
       <c r="M2" s="229"/>
       <c r="N2" s="229"/>
       <c r="O2" s="229"/>
-      <c r="P2" s="230"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="228"/>
+      <c r="Q2" s="228"/>
+      <c r="R2" s="228"/>
+      <c r="S2" s="228"/>
+      <c r="T2" s="228"/>
+      <c r="U2" s="228"/>
+      <c r="V2" s="228"/>
+      <c r="W2" s="228"/>
+      <c r="X2" s="228"/>
+      <c r="Y2" s="228"/>
+      <c r="Z2" s="228"/>
+      <c r="AA2" s="228"/>
+      <c r="AB2" s="228"/>
+      <c r="AC2" s="228"/>
+      <c r="AD2" s="228"/>
+      <c r="AE2" s="228"/>
+      <c r="AF2" s="228"/>
+      <c r="AG2" s="228"/>
+      <c r="AH2" s="228"/>
+      <c r="AI2" s="230"/>
+    </row>
+    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="231" t="s">
         <v>234</v>
       </c>
@@ -10866,9 +10886,28 @@
       <c r="M3" s="233"/>
       <c r="N3" s="233"/>
       <c r="O3" s="233"/>
-      <c r="P3" s="234"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P3" s="232"/>
+      <c r="Q3" s="232"/>
+      <c r="R3" s="232"/>
+      <c r="S3" s="232"/>
+      <c r="T3" s="232"/>
+      <c r="U3" s="232"/>
+      <c r="V3" s="232"/>
+      <c r="W3" s="232"/>
+      <c r="X3" s="232"/>
+      <c r="Y3" s="232"/>
+      <c r="Z3" s="232"/>
+      <c r="AA3" s="232"/>
+      <c r="AB3" s="232"/>
+      <c r="AC3" s="232"/>
+      <c r="AD3" s="232"/>
+      <c r="AE3" s="232"/>
+      <c r="AF3" s="232"/>
+      <c r="AG3" s="232"/>
+      <c r="AH3" s="232"/>
+      <c r="AI3" s="234"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D5" s="20" t="s">
         <v>10</v>
       </c>
@@ -10885,7 +10924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D6" s="26" t="s">
         <v>8</v>
       </c>
@@ -10899,8 +10938,31 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="13"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="27"/>
+      <c r="AI6" s="28"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D7" s="165">
         <v>0</v>
       </c>
@@ -10934,8 +10996,71 @@
       <c r="N7" s="225">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="14">
+        <v>11</v>
+      </c>
+      <c r="P7" s="15">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>13</v>
+      </c>
+      <c r="R7" s="15">
+        <v>14</v>
+      </c>
+      <c r="S7" s="15">
+        <v>15</v>
+      </c>
+      <c r="T7" s="14">
+        <v>16</v>
+      </c>
+      <c r="U7" s="15">
+        <v>17</v>
+      </c>
+      <c r="V7" s="15">
+        <v>18</v>
+      </c>
+      <c r="W7" s="15">
+        <v>19</v>
+      </c>
+      <c r="X7" s="15">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="15">
+        <v>21</v>
+      </c>
+      <c r="Z7" s="15">
+        <v>22</v>
+      </c>
+      <c r="AA7" s="15">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="14">
+        <v>24</v>
+      </c>
+      <c r="AC7" s="15">
+        <v>25</v>
+      </c>
+      <c r="AD7" s="15">
+        <v>26</v>
+      </c>
+      <c r="AE7" s="15">
+        <v>27</v>
+      </c>
+      <c r="AF7" s="16">
+        <v>28</v>
+      </c>
+      <c r="AG7" s="181">
+        <v>31</v>
+      </c>
+      <c r="AH7" s="182">
+        <v>30</v>
+      </c>
+      <c r="AI7" s="183">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D8" s="166" t="s">
         <v>107</v>
       </c>
@@ -10969,8 +11094,71 @@
       <c r="N8" s="171" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG8" s="184" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH8" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI8" s="186" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -11013,8 +11201,65 @@
       <c r="N10" s="67">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O10" s="67">
+        <v>1</v>
+      </c>
+      <c r="P10" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="67">
+        <v>1</v>
+      </c>
+      <c r="R10" s="67">
+        <v>1</v>
+      </c>
+      <c r="S10" s="67">
+        <v>1</v>
+      </c>
+      <c r="T10" s="67">
+        <v>1</v>
+      </c>
+      <c r="U10" s="67">
+        <v>1</v>
+      </c>
+      <c r="V10" s="67">
+        <v>1</v>
+      </c>
+      <c r="W10" s="67">
+        <v>1</v>
+      </c>
+      <c r="X10" s="67">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="67">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="67">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
         <v>239</v>
       </c>
@@ -11054,110 +11299,85 @@
       <c r="N11" s="67" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="91"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C13" t="s">
-        <v>236</v>
-      </c>
-      <c r="D13" s="67">
-        <v>0</v>
-      </c>
-      <c r="E13" s="67">
-        <v>1</v>
-      </c>
-      <c r="F13" s="67">
-        <v>1</v>
-      </c>
-      <c r="G13" s="67">
-        <v>1</v>
-      </c>
-      <c r="H13" s="67">
-        <v>1</v>
-      </c>
-      <c r="I13" s="67">
-        <v>0</v>
-      </c>
-      <c r="J13" s="67">
-        <v>0</v>
-      </c>
-      <c r="K13" s="67">
-        <v>0</v>
-      </c>
-      <c r="L13" s="67">
-        <v>0</v>
-      </c>
-      <c r="M13" s="67">
-        <v>0</v>
-      </c>
-      <c r="N13" s="67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="91" t="s">
-        <v>239</v>
-      </c>
-      <c r="C14" t="s">
-        <v>235</v>
-      </c>
-      <c r="D14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="67">
-        <v>1</v>
-      </c>
-      <c r="F14" s="67">
-        <v>1</v>
-      </c>
-      <c r="G14" s="67" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="L14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="M14" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" s="67" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="91"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="91"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="91"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
         <v>236</v>
       </c>
       <c r="D16" s="67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="67">
         <v>1</v>
@@ -11197,11 +11417,11 @@
       <c r="C17" t="s">
         <v>235</v>
       </c>
-      <c r="D17" s="67">
-        <v>1</v>
+      <c r="D17" s="67" t="s">
+        <v>46</v>
       </c>
       <c r="E17" s="67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="67">
         <v>1</v>
@@ -11242,7 +11462,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="67">
         <v>1</v>
@@ -11280,29 +11500,117 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="67">
+        <v>1</v>
+      </c>
+      <c r="E20" s="67">
+        <v>0</v>
+      </c>
+      <c r="F20" s="67">
+        <v>1</v>
+      </c>
+      <c r="G20" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="M20" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" s="67" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" s="67">
+        <v>1</v>
+      </c>
+      <c r="E22" s="67">
+        <v>1</v>
+      </c>
+      <c r="F22" s="67">
+        <v>1</v>
+      </c>
+      <c r="G22" s="67">
+        <v>1</v>
+      </c>
+      <c r="H22" s="67">
+        <v>1</v>
+      </c>
+      <c r="I22" s="67">
+        <v>0</v>
+      </c>
+      <c r="J22" s="67">
+        <v>0</v>
+      </c>
+      <c r="K22" s="67">
+        <v>0</v>
+      </c>
+      <c r="L22" s="67">
+        <v>0</v>
+      </c>
+      <c r="M22" s="67">
+        <v>0</v>
+      </c>
+      <c r="N22" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>238</v>
       </c>
-      <c r="D20" s="67">
-        <v>1</v>
-      </c>
-      <c r="E20" s="67">
-        <v>0</v>
-      </c>
-      <c r="F20" s="67">
-        <v>1</v>
-      </c>
-      <c r="G20" s="67">
-        <v>1</v>
-      </c>
-      <c r="H20" s="67">
+      <c r="D23" s="67">
+        <v>1</v>
+      </c>
+      <c r="E23" s="67">
+        <v>0</v>
+      </c>
+      <c r="F23" s="67">
+        <v>1</v>
+      </c>
+      <c r="G23" s="67">
+        <v>1</v>
+      </c>
+      <c r="H23" s="67">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D10:N10">
+  <conditionalFormatting sqref="D10:AI10">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -11314,7 +11622,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:N16">
+  <conditionalFormatting sqref="D19:N19">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -11326,7 +11634,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19:N19">
+  <conditionalFormatting sqref="D22:N22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -11338,7 +11646,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:N13">
+  <conditionalFormatting sqref="D16:N16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -12334,8 +12642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12417,7 +12725,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="221" t="str">
-        <f t="shared" ref="C3:C6" si="0">DEC2HEX(B3 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" ref="C3:C5" si="0">DEC2HEX(B3 + _xlfn.BITLSHIFT(B$2,8),4)</f>
         <v>0000</v>
       </c>
       <c r="D3" s="224" t="s">

</xml_diff>

<commit_message>
updated arch, updated library
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE0835E-67A2-4228-BDA3-9B6E2A5A52F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F397AA9C-6470-4F17-A146-F81A1D509F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="285">
   <si>
     <t>temperature</t>
   </si>
@@ -880,6 +880,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>with Q = 0 -&gt; error</t>
+  </si>
+  <si>
+    <t>with X = 0 -&gt; error</t>
+  </si>
+  <si>
+    <t>uptime shift</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1395,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="266">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2039,6 +2054,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2540,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABEE202-717B-4A96-9406-D9A14283F0F2}">
   <dimension ref="B1:AH50"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9036,8 +9055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36880ADF-04C9-4A12-8EFC-224812D037A0}">
   <dimension ref="A3:K87"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9106,7 +9125,9 @@
       <c r="I4" s="65">
         <v>8</v>
       </c>
-      <c r="K4" s="258"/>
+      <c r="K4" s="258" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="5" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
@@ -9268,7 +9289,9 @@
       <c r="I11" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="258"/>
+      <c r="K11" s="258" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
@@ -10840,7 +10863,7 @@
   <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="D10:H11"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11936,7 +11959,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12631,6 +12654,60 @@
       <c r="A16">
         <v>9</v>
       </c>
+      <c r="B16" s="212" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="96">
+        <v>0</v>
+      </c>
+      <c r="D16" s="97">
+        <v>0</v>
+      </c>
+      <c r="E16" s="58">
+        <v>0</v>
+      </c>
+      <c r="F16" s="96">
+        <v>1</v>
+      </c>
+      <c r="G16" s="97">
+        <v>1</v>
+      </c>
+      <c r="H16" s="96">
+        <v>0</v>
+      </c>
+      <c r="I16" s="264">
+        <v>1</v>
+      </c>
+      <c r="J16" s="264">
+        <v>0</v>
+      </c>
+      <c r="K16" s="264">
+        <v>0</v>
+      </c>
+      <c r="L16" s="264">
+        <v>0</v>
+      </c>
+      <c r="M16" s="97">
+        <v>0</v>
+      </c>
+      <c r="O16" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="P16" s="264" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q16" s="264" t="s">
+        <v>116</v>
+      </c>
+      <c r="R16" s="264" t="s">
+        <v>240</v>
+      </c>
+      <c r="S16" s="264" t="s">
+        <v>121</v>
+      </c>
+      <c r="T16" s="97" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -12664,10 +12741,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12676,16 +12753,17 @@
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="221" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="224" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" style="258" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>167</v>
       </c>
@@ -12698,39 +12776,40 @@
       <c r="D1" s="222" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="63"/>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="51"/>
+      <c r="M1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="218" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="217" t="s">
         <v>161</v>
       </c>
@@ -12739,12 +12818,15 @@
       </c>
       <c r="C2" s="220"/>
       <c r="D2" s="223"/>
-      <c r="H2" s="218">
-        <f>SUM(H3:H4)</f>
+      <c r="E2" s="265" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="218">
+        <f>SUM(I3:I4)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -12755,33 +12837,36 @@
       <c r="D3" s="224" t="s">
         <v>243</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="258">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>181</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3" si="0">F3*G3</f>
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3" si="0">G3*H3</f>
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
       <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>62</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -12792,134 +12877,161 @@
       <c r="D4" s="224" t="s">
         <v>244</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="258">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
         <v>245</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4" s="1">
-        <f>F4*G4</f>
+      <c r="I4" s="1">
+        <f>G4*H4</f>
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+      <c r="J4">
+        <v>1</v>
       </c>
       <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>65535</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>100</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="221" t="str">
-        <f>DEC2HEX(B5 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" ref="C5:C12" si="2">DEC2HEX(B5 + _xlfn.BITLSHIFT(B$2,8),4)</f>
         <v>0003</v>
       </c>
       <c r="D5" s="224" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="258">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>177</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H5" s="1">
-        <f>F5*G5</f>
+      <c r="I5" s="1">
+        <f>G5*H5</f>
         <v>32</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" s="221" t="str">
-        <f>DEC2HEX(B6 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>0004</v>
       </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E6" s="258">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" s="221" t="str">
-        <f>DEC2HEX(B7 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>0005</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E7" s="258">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" s="221" t="str">
-        <f>DEC2HEX(B8 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>0006</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="258">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" s="221" t="str">
-        <f>DEC2HEX(B9 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>0007</v>
       </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="258">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" s="221" t="str">
-        <f>DEC2HEX(B10 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>0008</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="258">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" s="221" t="str">
-        <f>DEC2HEX(B11 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>0009</v>
       </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="258">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" s="221" t="str">
-        <f>DEC2HEX(B12 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+        <f t="shared" si="2"/>
         <v>000A</v>
       </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="258">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="217" t="s">
         <v>160</v>
       </c>
@@ -12928,12 +13040,13 @@
       </c>
       <c r="C13" s="220"/>
       <c r="D13" s="223"/>
-      <c r="H13" s="218">
-        <f>SUM(H14:H18)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="265"/>
+      <c r="I13" s="218">
+        <f>SUM(I14:I19)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0</v>
       </c>
@@ -12944,234 +13057,280 @@
       <c r="D14" s="224" t="s">
         <v>165</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="258">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
         <v>178</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>4</v>
       </c>
-      <c r="H14" s="1">
-        <f>F14*G14</f>
+      <c r="I14" s="1">
+        <f>G14*H14</f>
         <v>4</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15">
-        <f>B14+ROUNDUP(H14/8,0)</f>
+        <f>B14+ROUNDUP(I14/8,0)</f>
         <v>1</v>
       </c>
       <c r="C15" s="221" t="str">
-        <f t="shared" ref="C15:C18" si="2">DEC2HEX(B15 + _xlfn.BITLSHIFT(B$13,8),4)</f>
+        <f t="shared" ref="C15:C19" si="3">DEC2HEX(B15 + _xlfn.BITLSHIFT(B$13,8),4)</f>
         <v>0101</v>
       </c>
       <c r="D15" s="224" t="s">
         <v>271</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="258">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>178</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
-        <f>F15*G15</f>
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1">
+        <f>G15*H15</f>
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
-        <f t="shared" ref="B16:B18" si="3">B15+ROUNDUP(H15/8,0)</f>
         <v>2</v>
       </c>
       <c r="C16" s="221" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0102</v>
       </c>
       <c r="D16" s="224" t="s">
+        <v>284</v>
+      </c>
+      <c r="E16" s="258">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1">
+        <f>G16*H16</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="221" t="str">
+        <f t="shared" si="3"/>
+        <v>0103</v>
+      </c>
+      <c r="D17" s="224" t="s">
         <v>273</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" s="258">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
         <v>178</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>4</v>
       </c>
-      <c r="H16" s="1">
-        <f t="shared" ref="H16:H17" si="4">F16*G16</f>
+      <c r="I17" s="1">
+        <f t="shared" ref="I17:I18" si="4">G17*H17</f>
         <v>4</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" s="221" t="str">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="C17" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>0103</v>
-      </c>
-      <c r="D17" s="224" t="s">
+        <v>0104</v>
+      </c>
+      <c r="D18" s="224" t="s">
         <v>274</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" s="258">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
         <v>178</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>4</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I18" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="221" t="str">
         <f t="shared" si="3"/>
+        <v>0105</v>
+      </c>
+      <c r="D19" s="224" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="258">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>181</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <f>G19*H19</f>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19">
+        <v>35</v>
+      </c>
+      <c r="P19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="217" t="s">
+        <v>252</v>
+      </c>
+      <c r="B22" s="218">
+        <v>2</v>
+      </c>
+      <c r="C22" s="220"/>
+      <c r="D22" s="223"/>
+      <c r="E22" s="265"/>
+      <c r="I22" s="218">
+        <f>SUM(I23:I24)</f>
         <v>4</v>
       </c>
-      <c r="C18" s="221" t="str">
-        <f t="shared" si="2"/>
-        <v>0104</v>
-      </c>
-      <c r="D18" s="224" t="s">
-        <v>180</v>
-      </c>
-      <c r="E18" t="s">
-        <v>181</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
-        <f>F18*G18</f>
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>100</v>
-      </c>
-      <c r="N18">
-        <v>35</v>
-      </c>
-      <c r="O18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="217" t="s">
-        <v>252</v>
-      </c>
-      <c r="B21" s="218">
-        <v>2</v>
-      </c>
-      <c r="C21" s="220"/>
-      <c r="D21" s="223"/>
-      <c r="H21" s="218">
-        <f>SUM(H22:H23)</f>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="221" t="str">
+        <f>DEC2HEX(B23 + _xlfn.BITLSHIFT(B$22,8),4)</f>
+        <v>0200</v>
+      </c>
+      <c r="D23" s="224" t="s">
+        <v>275</v>
+      </c>
+      <c r="E23" s="258">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="221" t="str">
-        <f>DEC2HEX(B22 + _xlfn.BITLSHIFT(B$21,8),4)</f>
-        <v>0200</v>
-      </c>
-      <c r="D22" s="224" t="s">
-        <v>275</v>
-      </c>
-      <c r="E22" t="s">
-        <v>178</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
+      <c r="I23" s="1">
+        <f>G23*H23</f>
         <v>4</v>
       </c>
-      <c r="H22" s="1">
-        <f>F22*G22</f>
-        <v>4</v>
-      </c>
-      <c r="O22" t="s">
+      <c r="P23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="221" t="str">
-        <f t="shared" ref="C23" si="5">DEC2HEX(B23 + _xlfn.BITLSHIFT(B$21,8),4)</f>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="221" t="str">
+        <f t="shared" ref="C24" si="5">DEC2HEX(B24 + _xlfn.BITLSHIFT(B$22,8),4)</f>
         <v>0201</v>
       </c>
-      <c r="H23" s="1">
-        <f>F23*G23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="217" t="s">
+      <c r="I24" s="1">
+        <f>G24*H24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="217" t="s">
         <v>272</v>
       </c>
-      <c r="B30" s="218">
+      <c r="B31" s="218">
         <v>3</v>
       </c>
-      <c r="C30" s="220"/>
-      <c r="D30" s="223"/>
-      <c r="H30" s="218">
-        <f>SUM(H31:H32)</f>
+      <c r="C31" s="220"/>
+      <c r="D31" s="223"/>
+      <c r="E31" s="265"/>
+      <c r="I31" s="218">
+        <f>SUM(I32:I33)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changed device_identification section location + linker script
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F397AA9C-6470-4F17-A146-F81A1D509F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09464772-404B-4012-9DB8-A9B85A736E6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="308">
   <si>
     <t>temperature</t>
   </si>
@@ -798,9 +798,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>TELEMETRY CONFIG</t>
-  </si>
-  <si>
     <t>Data type</t>
   </si>
   <si>
@@ -855,18 +852,9 @@
     <t>OutdoorSensor1</t>
   </si>
   <si>
-    <t>abs time</t>
-  </si>
-  <si>
     <t>SCHEDULE</t>
   </si>
   <si>
-    <t>messages sent</t>
-  </si>
-  <si>
-    <t>messages received</t>
-  </si>
-  <si>
     <t>telemetry period</t>
   </si>
   <si>
@@ -894,14 +882,95 @@
     <t>with X = 0 -&gt; error</t>
   </si>
   <si>
-    <t>uptime shift</t>
+    <t>FLASH</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>CONFIG</t>
+  </si>
+  <si>
+    <t>0 (disabled)</t>
+  </si>
+  <si>
+    <t>UINT32_MAX</t>
+  </si>
+  <si>
+    <t>last_telemetry</t>
+  </si>
+  <si>
+    <t>message_sent</t>
+  </si>
+  <si>
+    <t>message_received</t>
+  </si>
+  <si>
+    <t>uptime_shift</t>
+  </si>
+  <si>
+    <t>abstime</t>
+  </si>
+  <si>
+    <t>schedule[1] days</t>
+  </si>
+  <si>
+    <t>schedule[0] days</t>
+  </si>
+  <si>
+    <t>schedule[0] time</t>
+  </si>
+  <si>
+    <t>schedule[0] controller</t>
+  </si>
+  <si>
+    <t>schedule[2] time</t>
+  </si>
+  <si>
+    <t>schedule[1] time</t>
+  </si>
+  <si>
+    <t>schedule[1] controller</t>
+  </si>
+  <si>
+    <t>schedule[2] days</t>
+  </si>
+  <si>
+    <t>schedule[2] controller</t>
+  </si>
+  <si>
+    <t>schedule[3] days</t>
+  </si>
+  <si>
+    <t>schedule[3] time</t>
+  </si>
+  <si>
+    <t>schedule[3] controller</t>
+  </si>
+  <si>
+    <t>schedule[4] days</t>
+  </si>
+  <si>
+    <t>schedule[4] time</t>
+  </si>
+  <si>
+    <t>schedule[4] controller</t>
+  </si>
+  <si>
+    <t>1*</t>
+  </si>
+  <si>
+    <t>TELEMETRY/SCHEDULE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -989,6 +1058,14 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1395,7 +1472,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="266">
+  <cellXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2058,6 +2135,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2559,7 +2639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABEE202-717B-4A96-9406-D9A14283F0F2}">
   <dimension ref="B1:AH50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
@@ -3718,7 +3798,7 @@
         <v>154</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -4284,7 +4364,7 @@
         <v>153</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
@@ -4297,7 +4377,7 @@
       <c r="L40" s="48"/>
       <c r="M40" s="48"/>
       <c r="T40" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="2:34" x14ac:dyDescent="0.2">
@@ -4327,7 +4407,7 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="19" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>145</v>
@@ -4860,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D135A44-A127-4252-B653-8392D6AD3A28}">
   <dimension ref="A2:BO45"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4875,7 +4955,7 @@
   <sheetData>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>157</v>
@@ -4966,7 +5046,7 @@
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A3" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>84</v>
@@ -5171,207 +5251,207 @@
     <row r="4" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A4" s="247"/>
       <c r="B4" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C4" s="241">
         <v>8</v>
       </c>
       <c r="D4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="R4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="S4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="W4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="X4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Y4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AB4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AC4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AD4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AE4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AG4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AH4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AI4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AJ4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AK4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AL4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AM4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AN4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AO4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AP4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AQ4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AR4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AS4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AT4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AU4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AV4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AW4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AX4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AY4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AZ4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BA4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BB4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BC4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BD4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BE4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BF4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BG4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BH4" s="243" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BI4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BJ4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BK4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BL4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BM4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BN4" s="244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BO4" s="245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A6" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>157</v>
@@ -5462,7 +5542,7 @@
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A7" s="248" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>83</v>
@@ -5667,7 +5747,7 @@
     <row r="8" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A8" s="247"/>
       <c r="B8" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" s="241">
         <v>1</v>
@@ -5867,7 +5947,7 @@
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A10" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>157</v>
@@ -5958,7 +6038,7 @@
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A11" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>83</v>
@@ -6163,7 +6243,7 @@
     <row r="12" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A12" s="247"/>
       <c r="B12" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" s="241">
         <v>4</v>
@@ -6217,34 +6297,34 @@
         <v>42</v>
       </c>
       <c r="T12" s="187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="V12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="W12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="X12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Z12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AA12" s="240" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AB12" s="187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AC12" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AD12" s="185" t="s">
         <v>46</v>
@@ -6397,7 +6477,7 @@
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A14" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>157</v>
@@ -6488,7 +6568,7 @@
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A15" s="249" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>84</v>
@@ -6693,7 +6773,7 @@
     <row r="16" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A16" s="247"/>
       <c r="B16" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C16" s="241">
         <v>4</v>
@@ -6927,7 +7007,7 @@
     </row>
     <row r="18" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A18" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>157</v>
@@ -7018,7 +7098,7 @@
     </row>
     <row r="19" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A19" s="249" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>84</v>
@@ -7223,7 +7303,7 @@
     <row r="20" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A20" s="247"/>
       <c r="B20" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="241">
         <v>8</v>
@@ -7373,34 +7453,34 @@
         <v>25</v>
       </c>
       <c r="AZ20" s="187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BA20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BB20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BC20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BD20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BE20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BF20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BG20" s="240" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BH20" s="187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BI20" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BJ20" s="185" t="s">
         <v>46</v>
@@ -7457,7 +7537,7 @@
     </row>
     <row r="22" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A22" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>157</v>
@@ -7548,7 +7628,7 @@
     </row>
     <row r="23" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A23" s="249" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>84</v>
@@ -7677,83 +7757,83 @@
       <c r="AQ23" s="24">
         <v>39</v>
       </c>
-      <c r="AR23" s="23">
+      <c r="AR23" s="263">
         <v>40</v>
       </c>
-      <c r="AS23" s="19">
+      <c r="AS23" s="18">
         <v>41</v>
       </c>
-      <c r="AT23" s="19">
+      <c r="AT23" s="18">
         <v>42</v>
       </c>
-      <c r="AU23" s="19">
+      <c r="AU23" s="18">
         <v>43</v>
       </c>
-      <c r="AV23" s="19">
+      <c r="AV23" s="18">
         <v>44</v>
       </c>
-      <c r="AW23" s="19">
+      <c r="AW23" s="18">
         <v>45</v>
       </c>
-      <c r="AX23" s="19">
-        <v>46</v>
-      </c>
-      <c r="AY23" s="24">
+      <c r="AX23" s="18">
+        <v>46</v>
+      </c>
+      <c r="AY23" s="209">
         <v>47</v>
       </c>
-      <c r="AZ23" s="23">
+      <c r="AZ23" s="263">
         <v>48</v>
       </c>
-      <c r="BA23" s="19">
+      <c r="BA23" s="18">
         <v>49</v>
       </c>
-      <c r="BB23" s="19">
+      <c r="BB23" s="18">
         <v>50</v>
       </c>
-      <c r="BC23" s="19">
+      <c r="BC23" s="18">
         <v>51</v>
       </c>
-      <c r="BD23" s="19">
+      <c r="BD23" s="18">
         <v>52</v>
       </c>
-      <c r="BE23" s="19">
+      <c r="BE23" s="18">
         <v>53</v>
       </c>
-      <c r="BF23" s="19">
+      <c r="BF23" s="18">
         <v>54</v>
       </c>
-      <c r="BG23" s="24">
+      <c r="BG23" s="209">
         <v>55</v>
       </c>
-      <c r="BH23" s="23">
+      <c r="BH23" s="263">
         <v>56</v>
       </c>
-      <c r="BI23" s="19">
+      <c r="BI23" s="18">
         <v>57</v>
       </c>
-      <c r="BJ23" s="19">
+      <c r="BJ23" s="18">
         <v>58</v>
       </c>
-      <c r="BK23" s="19">
+      <c r="BK23" s="18">
         <v>59</v>
       </c>
-      <c r="BL23" s="19">
+      <c r="BL23" s="18">
         <v>60</v>
       </c>
-      <c r="BM23" s="19">
+      <c r="BM23" s="18">
         <v>61</v>
       </c>
-      <c r="BN23" s="19">
+      <c r="BN23" s="18">
         <v>62</v>
       </c>
-      <c r="BO23" s="24">
+      <c r="BO23" s="209">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A24" s="247"/>
       <c r="B24" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C24" s="241">
         <v>8</v>
@@ -7855,105 +7935,105 @@
         <v>24</v>
       </c>
       <c r="AJ24" s="187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AK24" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AL24" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AM24" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AN24" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AO24" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AP24" s="188" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AQ24" s="240" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AR24" s="187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AS24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="AT24" s="185" t="s">
-        <v>46</v>
+        <v>254</v>
+      </c>
+      <c r="AT24" s="188" t="s">
+        <v>258</v>
       </c>
       <c r="AU24" s="188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AV24" s="188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AW24" s="188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AX24" s="188" t="s">
-        <v>259</v>
-      </c>
-      <c r="AY24" s="240" t="s">
-        <v>259</v>
+        <v>258</v>
+      </c>
+      <c r="AY24" s="188" t="s">
+        <v>258</v>
       </c>
       <c r="AZ24" s="187" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BA24" s="188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BB24" s="188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BC24" s="188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BD24" s="188" t="s">
         <v>259</v>
       </c>
-      <c r="BE24" s="185" t="s">
-        <v>46</v>
+      <c r="BE24" s="188" t="s">
+        <v>259</v>
       </c>
       <c r="BF24" s="188" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BG24" s="240" t="s">
-        <v>260</v>
-      </c>
-      <c r="BH24" s="187" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="BH24" s="188" t="s">
+        <v>259</v>
       </c>
       <c r="BI24" s="188" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BJ24" s="188" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BK24" s="188" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BL24" s="188" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BM24" s="188" t="s">
-        <v>260</v>
-      </c>
-      <c r="BN24" s="188" t="s">
-        <v>260</v>
-      </c>
-      <c r="BO24" s="240" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="BN24" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="BO24" s="186" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A26" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>157</v>
@@ -8044,7 +8124,7 @@
     </row>
     <row r="27" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A27" s="249" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>84</v>
@@ -8249,7 +8329,7 @@
     <row r="28" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A28" s="247"/>
       <c r="B28" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C28" s="241">
         <v>8</v>
@@ -8399,52 +8479,52 @@
         <v>26</v>
       </c>
       <c r="AZ28" s="39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BA28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BB28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BC28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BD28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BE28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BF28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BG28" s="41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BH28" s="39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BI28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BJ28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BK28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BL28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BM28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BN28" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BO28" s="41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:67" x14ac:dyDescent="0.2">
@@ -8483,7 +8563,7 @@
     </row>
     <row r="30" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A30" s="246" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>157</v>
@@ -8779,7 +8859,7 @@
     <row r="32" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A32" s="247"/>
       <c r="B32" s="237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C32" s="241">
         <v>0</v>
@@ -9056,7 +9136,7 @@
   <dimension ref="A3:K87"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9126,7 +9206,7 @@
         <v>8</v>
       </c>
       <c r="K4" s="258" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9290,7 +9370,7 @@
         <v>45</v>
       </c>
       <c r="K11" s="258" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9514,10 +9594,10 @@
         <v>58</v>
       </c>
       <c r="I23" s="64" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K23" s="259" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9576,7 +9656,7 @@
         <v>85</v>
       </c>
       <c r="I25" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K25" s="260"/>
     </row>
@@ -9604,7 +9684,7 @@
       </c>
       <c r="H26" s="86"/>
       <c r="I26" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K26" s="260"/>
     </row>
@@ -9627,7 +9707,7 @@
       </c>
       <c r="H27" s="86"/>
       <c r="I27" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K27" s="260"/>
     </row>
@@ -9648,7 +9728,7 @@
       </c>
       <c r="H28" s="88"/>
       <c r="I28" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K28" s="261"/>
     </row>
@@ -9669,7 +9749,7 @@
       </c>
       <c r="H29" s="88"/>
       <c r="I29" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K29" s="261"/>
     </row>
@@ -9690,7 +9770,7 @@
       </c>
       <c r="H30" s="88"/>
       <c r="I30" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K30" s="261"/>
     </row>
@@ -9711,7 +9791,7 @@
       </c>
       <c r="H31" s="88"/>
       <c r="I31" s="250" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K31" s="261"/>
     </row>
@@ -9732,10 +9812,10 @@
       </c>
       <c r="H32" s="88"/>
       <c r="I32" s="251" t="s">
+        <v>266</v>
+      </c>
+      <c r="K32" s="261" t="s">
         <v>267</v>
-      </c>
-      <c r="K32" s="261" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.25">
@@ -9755,7 +9835,7 @@
       </c>
       <c r="H33" s="88"/>
       <c r="I33" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K33" s="261"/>
     </row>
@@ -9776,7 +9856,7 @@
       </c>
       <c r="H34" s="88"/>
       <c r="I34" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K34" s="261"/>
     </row>
@@ -9797,7 +9877,7 @@
       </c>
       <c r="H35" s="88"/>
       <c r="I35" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K35" s="261"/>
     </row>
@@ -9818,7 +9898,7 @@
       </c>
       <c r="H36" s="88"/>
       <c r="I36" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K36" s="261"/>
     </row>
@@ -9839,7 +9919,7 @@
       </c>
       <c r="H37" s="88"/>
       <c r="I37" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K37" s="261"/>
     </row>
@@ -9860,7 +9940,7 @@
       </c>
       <c r="H38" s="85"/>
       <c r="I38" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K38" s="261"/>
     </row>
@@ -9881,7 +9961,7 @@
       </c>
       <c r="H39" s="89"/>
       <c r="I39" s="251" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K39" s="261"/>
     </row>
@@ -9901,7 +9981,7 @@
         <v>182</v>
       </c>
       <c r="I40" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K40" s="261"/>
     </row>
@@ -9921,7 +10001,7 @@
         <v>183</v>
       </c>
       <c r="I41" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K41" s="261"/>
     </row>
@@ -9941,7 +10021,7 @@
         <v>184</v>
       </c>
       <c r="I42" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K42" s="261"/>
     </row>
@@ -9961,7 +10041,7 @@
         <v>185</v>
       </c>
       <c r="I43" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K43" s="261"/>
     </row>
@@ -9981,7 +10061,7 @@
         <v>186</v>
       </c>
       <c r="I44" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K44" s="261"/>
     </row>
@@ -10001,7 +10081,7 @@
         <v>187</v>
       </c>
       <c r="I45" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K45" s="261"/>
     </row>
@@ -10021,7 +10101,7 @@
         <v>188</v>
       </c>
       <c r="I46" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K46" s="261"/>
     </row>
@@ -10041,7 +10121,7 @@
         <v>189</v>
       </c>
       <c r="I47" s="252" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K47" s="261"/>
     </row>
@@ -10061,10 +10141,10 @@
         <v>190</v>
       </c>
       <c r="I48" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K48" s="261" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
@@ -10083,7 +10163,7 @@
         <v>191</v>
       </c>
       <c r="I49" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K49" s="261"/>
     </row>
@@ -10103,7 +10183,7 @@
         <v>192</v>
       </c>
       <c r="I50" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K50" s="261"/>
     </row>
@@ -10123,7 +10203,7 @@
         <v>193</v>
       </c>
       <c r="I51" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K51" s="261"/>
     </row>
@@ -10143,7 +10223,7 @@
         <v>194</v>
       </c>
       <c r="I52" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K52" s="261"/>
     </row>
@@ -10163,7 +10243,7 @@
         <v>195</v>
       </c>
       <c r="I53" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K53" s="261"/>
     </row>
@@ -10183,7 +10263,7 @@
         <v>196</v>
       </c>
       <c r="I54" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K54" s="261"/>
     </row>
@@ -10203,7 +10283,7 @@
         <v>197</v>
       </c>
       <c r="I55" s="251" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K55" s="261"/>
     </row>
@@ -10223,7 +10303,7 @@
         <v>198</v>
       </c>
       <c r="I56" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K56" s="261"/>
     </row>
@@ -10243,7 +10323,7 @@
         <v>199</v>
       </c>
       <c r="I57" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K57" s="261"/>
     </row>
@@ -10263,7 +10343,7 @@
         <v>200</v>
       </c>
       <c r="I58" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K58" s="261"/>
     </row>
@@ -10283,7 +10363,7 @@
         <v>201</v>
       </c>
       <c r="I59" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K59" s="261"/>
     </row>
@@ -10303,7 +10383,7 @@
         <v>202</v>
       </c>
       <c r="I60" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K60" s="261"/>
     </row>
@@ -10323,7 +10403,7 @@
         <v>203</v>
       </c>
       <c r="I61" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K61" s="261"/>
     </row>
@@ -10343,7 +10423,7 @@
         <v>204</v>
       </c>
       <c r="I62" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K62" s="261"/>
     </row>
@@ -10363,7 +10443,7 @@
         <v>205</v>
       </c>
       <c r="I63" s="251" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K63" s="261"/>
     </row>
@@ -10383,7 +10463,7 @@
         <v>206</v>
       </c>
       <c r="I64" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K64" s="261"/>
     </row>
@@ -10403,7 +10483,7 @@
         <v>207</v>
       </c>
       <c r="I65" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K65" s="261"/>
     </row>
@@ -10423,7 +10503,7 @@
         <v>208</v>
       </c>
       <c r="I66" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K66" s="261"/>
     </row>
@@ -10443,7 +10523,7 @@
         <v>209</v>
       </c>
       <c r="I67" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K67" s="261"/>
     </row>
@@ -10463,7 +10543,7 @@
         <v>210</v>
       </c>
       <c r="I68" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K68" s="261"/>
     </row>
@@ -10483,7 +10563,7 @@
         <v>211</v>
       </c>
       <c r="I69" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K69" s="261"/>
     </row>
@@ -10503,7 +10583,7 @@
         <v>212</v>
       </c>
       <c r="I70" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K70" s="261"/>
     </row>
@@ -10523,7 +10603,7 @@
         <v>213</v>
       </c>
       <c r="I71" s="251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K71" s="261"/>
     </row>
@@ -10543,7 +10623,7 @@
         <v>214</v>
       </c>
       <c r="I72" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K72" s="261"/>
     </row>
@@ -10563,7 +10643,7 @@
         <v>215</v>
       </c>
       <c r="I73" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K73" s="261"/>
     </row>
@@ -10583,7 +10663,7 @@
         <v>216</v>
       </c>
       <c r="I74" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K74" s="261"/>
     </row>
@@ -10603,7 +10683,7 @@
         <v>217</v>
       </c>
       <c r="I75" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K75" s="261"/>
     </row>
@@ -10623,7 +10703,7 @@
         <v>218</v>
       </c>
       <c r="I76" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K76" s="261"/>
     </row>
@@ -10643,7 +10723,7 @@
         <v>219</v>
       </c>
       <c r="I77" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K77" s="261"/>
     </row>
@@ -10663,7 +10743,7 @@
         <v>220</v>
       </c>
       <c r="I78" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K78" s="261"/>
     </row>
@@ -10683,7 +10763,7 @@
         <v>221</v>
       </c>
       <c r="I79" s="251" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K79" s="261"/>
     </row>
@@ -11791,10 +11871,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="239" t="s">
         <v>256</v>
-      </c>
-      <c r="C7" s="239" t="s">
-        <v>257</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -11959,7 +12039,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12655,7 +12735,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="212" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C16" s="96">
         <v>0</v>
@@ -12694,7 +12774,7 @@
         <v>105</v>
       </c>
       <c r="P16" s="264" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q16" s="264" t="s">
         <v>116</v>
@@ -12709,27 +12789,60 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" s="96">
+        <v>1</v>
+      </c>
+      <c r="D17" s="97">
+        <v>0</v>
+      </c>
+      <c r="E17" s="58">
+        <v>1</v>
+      </c>
+      <c r="F17" s="96">
+        <v>1</v>
+      </c>
+      <c r="G17" s="97">
+        <v>1</v>
+      </c>
+      <c r="H17" s="96">
+        <v>0</v>
+      </c>
+      <c r="I17" s="264">
+        <v>1</v>
+      </c>
+      <c r="J17" s="264">
+        <v>1</v>
+      </c>
+      <c r="K17" s="264">
+        <v>0</v>
+      </c>
+      <c r="L17" s="264">
+        <v>0</v>
+      </c>
+      <c r="M17" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
@@ -12741,591 +12854,926 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="221" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="224" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" style="258" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="221" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="224" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="258" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="219" t="s">
+      <c r="E1" s="219" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="222" t="s">
+      <c r="F1" s="222" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="63"/>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="J1" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="M1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="51"/>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="51"/>
+      <c r="O1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="218" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="217" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="218">
-        <v>0</v>
-      </c>
-      <c r="C2" s="220"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="265" t="s">
+      <c r="C2" s="218" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="218">
+        <v>0</v>
+      </c>
+      <c r="E2" s="220"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="265" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="218">
-        <f>SUM(I3:I4)</f>
+      <c r="K2" s="218">
+        <f>SUM(K3:K4)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="221" t="str">
-        <f>DEC2HEX(B3 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="221" t="str">
+        <f>DEC2HEX(D3 + _xlfn.BITLSHIFT(D$2,8),4)</f>
         <v>0000</v>
       </c>
-      <c r="D3" s="224" t="s">
+      <c r="F3" s="224" t="s">
         <v>243</v>
       </c>
-      <c r="E3" s="258">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" s="258">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>181</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3" si="0">G3*H3</f>
+      <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
+      <c r="K3" s="1">
+        <f t="shared" ref="K3" si="0">I3*J3</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
         <v>62</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="221" t="str">
-        <f t="shared" ref="C4" si="1">DEC2HEX(B4 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="221" t="str">
+        <f t="shared" ref="E4" si="1">DEC2HEX(D4 + _xlfn.BITLSHIFT(D$2,8),4)</f>
         <v>0001</v>
       </c>
-      <c r="D4" s="224" t="s">
+      <c r="F4" s="224" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="258">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" s="258">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>245</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="I4" s="1">
-        <f>G4*H4</f>
+      <c r="K4" s="1">
+        <f>I4*J4</f>
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>65535</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>100</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="C5" s="221" t="str">
-        <f t="shared" ref="C5:C12" si="2">DEC2HEX(B5 + _xlfn.BITLSHIFT(B$2,8),4)</f>
+      <c r="E5" s="221" t="str">
+        <f t="shared" ref="E5:E12" si="2">DEC2HEX(D5 + _xlfn.BITLSHIFT(D$2,8),4)</f>
         <v>0003</v>
       </c>
-      <c r="D5" s="224" t="s">
+      <c r="F5" s="224" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="258">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" s="258">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>177</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>8</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="I5" s="1">
-        <f>G5*H5</f>
+      <c r="K5" s="1">
+        <f>I5*J5</f>
         <v>32</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="C6" s="221" t="str">
+      <c r="E6" s="221" t="str">
         <f t="shared" si="2"/>
         <v>0004</v>
       </c>
-      <c r="E6" s="258">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="F6" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="258">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="C7" s="221" t="str">
+      <c r="E7" s="221" t="str">
         <f t="shared" si="2"/>
         <v>0005</v>
       </c>
-      <c r="E7" s="258">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="F7" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="258">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8">
         <v>6</v>
       </c>
-      <c r="C8" s="221" t="str">
+      <c r="E8" s="221" t="str">
         <f t="shared" si="2"/>
         <v>0006</v>
       </c>
-      <c r="E8" s="258">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="F8" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="258">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="C9" s="221" t="str">
+      <c r="E9" s="221" t="str">
         <f t="shared" si="2"/>
         <v>0007</v>
       </c>
-      <c r="E9" s="258">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="F9" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="258">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="C10" s="221" t="str">
+      <c r="E10" s="221" t="str">
         <f t="shared" si="2"/>
         <v>0008</v>
       </c>
-      <c r="E10" s="258">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="F10" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="258">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="C11" s="221" t="str">
+      <c r="E11" s="221" t="str">
         <f t="shared" si="2"/>
         <v>0009</v>
       </c>
-      <c r="E11" s="258">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="F11" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="258">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="C12" s="221" t="str">
+      <c r="E12" s="221" t="str">
         <f t="shared" si="2"/>
         <v>000A</v>
       </c>
-      <c r="E12" s="258">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="217" t="s">
+      <c r="F12" s="224" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="258">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="258">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="217" t="s">
         <v>160</v>
       </c>
-      <c r="B13" s="218">
-        <v>1</v>
-      </c>
-      <c r="C13" s="220"/>
-      <c r="D13" s="223"/>
-      <c r="E13" s="265"/>
-      <c r="I13" s="218">
-        <f>SUM(I14:I19)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="221" t="str">
-        <f>DEC2HEX(B14 + _xlfn.BITLSHIFT(B$13,8),4)</f>
+      <c r="C14" s="218" t="s">
+        <v>282</v>
+      </c>
+      <c r="D14" s="218">
+        <v>1</v>
+      </c>
+      <c r="E14" s="220"/>
+      <c r="F14" s="223"/>
+      <c r="G14" s="265"/>
+      <c r="K14" s="218">
+        <f>SUM(K15:K21)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="221" t="str">
+        <f>DEC2HEX(D15 + _xlfn.BITLSHIFT(D$14,8),4)</f>
         <v>0100</v>
       </c>
-      <c r="D14" s="224" t="s">
+      <c r="F15" s="224" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="258">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G15" s="258">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>178</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
         <v>4</v>
       </c>
-      <c r="I14" s="1">
-        <f>G14*H14</f>
+      <c r="K15" s="1">
+        <f>I15*J15</f>
         <v>4</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <f>B14+ROUNDUP(I14/8,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="221" t="str">
-        <f t="shared" ref="C15:C19" si="3">DEC2HEX(B15 + _xlfn.BITLSHIFT(B$13,8),4)</f>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f>D15+ROUNDUP(K15/8,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="221" t="str">
+        <f>DEC2HEX(D16 + _xlfn.BITLSHIFT(D$14,8),4)</f>
         <v>0101</v>
       </c>
-      <c r="D15" s="224" t="s">
-        <v>271</v>
-      </c>
-      <c r="E15" s="258">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F16" s="224" t="s">
+        <v>290</v>
+      </c>
+      <c r="G16" s="258">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>178</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
         <v>4</v>
       </c>
-      <c r="I15" s="1">
-        <f>G15*H15</f>
+      <c r="K16" s="1">
+        <f>I16*J16</f>
         <v>4</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="C16" s="221" t="str">
-        <f t="shared" si="3"/>
+      <c r="E17" s="221" t="str">
+        <f t="shared" ref="E17:E21" si="3">DEC2HEX(D17 + _xlfn.BITLSHIFT(D$14,8),4)</f>
         <v>0102</v>
       </c>
-      <c r="D16" s="224" t="s">
-        <v>284</v>
-      </c>
-      <c r="E16" s="258">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="F17" s="224" t="s">
+        <v>289</v>
+      </c>
+      <c r="G17" s="266" t="s">
+        <v>306</v>
+      </c>
+      <c r="H17" t="s">
         <v>178</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
         <v>4</v>
       </c>
-      <c r="I16" s="1">
-        <f>G16*H16</f>
+      <c r="K17" s="1">
+        <f>I17*J17</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" ref="D18" si="4">D17+ROUNDUP(K17/8,0)</f>
         <v>3</v>
       </c>
-      <c r="C17" s="221" t="str">
+      <c r="E18" s="221" t="str">
         <f t="shared" si="3"/>
         <v>0103</v>
       </c>
-      <c r="D17" s="224" t="s">
-        <v>273</v>
-      </c>
-      <c r="E17" s="258">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="F18" s="224" t="s">
+        <v>286</v>
+      </c>
+      <c r="G18" s="258">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>178</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
         <v>4</v>
       </c>
-      <c r="I17" s="1">
-        <f t="shared" ref="I17:I18" si="4">G17*H17</f>
+      <c r="K18" s="1">
         <v>4</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="221" t="str">
+        <f t="shared" si="3"/>
+        <v>0103</v>
+      </c>
+      <c r="F19" s="224" t="s">
+        <v>287</v>
+      </c>
+      <c r="G19" s="258">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
         <v>4</v>
       </c>
-      <c r="C18" s="221" t="str">
+      <c r="K19" s="1">
+        <f t="shared" ref="K19:K20" si="5">I19*J19</f>
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" ref="D20" si="6">D19+ROUNDUP(K19/8,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E20" s="221" t="str">
         <f t="shared" si="3"/>
         <v>0104</v>
       </c>
-      <c r="D18" s="224" t="s">
-        <v>274</v>
-      </c>
-      <c r="E18" s="258">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="F20" s="224" t="s">
+        <v>288</v>
+      </c>
+      <c r="G20" s="258">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
         <v>178</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
         <v>4</v>
       </c>
-      <c r="I18" s="1">
-        <f t="shared" si="4"/>
+      <c r="K20" s="1">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="221" t="str">
+        <f t="shared" si="3"/>
+        <v>0104</v>
+      </c>
+      <c r="F21" s="224" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="258">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>181</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1">
+        <f>I21*J21</f>
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>100</v>
+      </c>
+      <c r="Q21">
+        <v>35</v>
+      </c>
+      <c r="R21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" ref="D22" si="7">D21+ROUNDUP(K21/8,0)</f>
         <v>5</v>
       </c>
-      <c r="C19" s="221" t="str">
-        <f t="shared" si="3"/>
-        <v>0105</v>
-      </c>
-      <c r="D19" s="224" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="258">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>181</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1">
-        <f>G19*H19</f>
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>100</v>
-      </c>
-      <c r="O19">
-        <v>35</v>
-      </c>
-      <c r="P19" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="217" t="s">
-        <v>252</v>
-      </c>
-      <c r="B22" s="218">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="217" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="218" t="s">
+        <v>307</v>
+      </c>
+      <c r="C24" s="218" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" s="218">
         <v>2</v>
       </c>
-      <c r="C22" s="220"/>
-      <c r="D22" s="223"/>
-      <c r="E22" s="265"/>
-      <c r="I22" s="218">
-        <f>SUM(I23:I24)</f>
+      <c r="E24" s="220"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="265"/>
+      <c r="K24" s="218">
+        <f>SUM(K25:K26)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="221" t="str">
-        <f>DEC2HEX(B23 + _xlfn.BITLSHIFT(B$22,8),4)</f>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="221" t="str">
+        <f>DEC2HEX(D25 + _xlfn.BITLSHIFT(D$24,8),4)</f>
         <v>0200</v>
       </c>
-      <c r="D23" s="224" t="s">
-        <v>275</v>
-      </c>
-      <c r="E23" s="258">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="F25" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="G25" s="258">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
         <v>178</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
         <v>4</v>
       </c>
-      <c r="I23" s="1">
-        <f>G23*H23</f>
+      <c r="K25" s="1">
+        <f>I25*J25</f>
         <v>4</v>
       </c>
-      <c r="P23" t="s">
+      <c r="O25" t="s">
+        <v>284</v>
+      </c>
+      <c r="P25" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q25">
+        <v>10</v>
+      </c>
+      <c r="R25" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="221" t="str">
-        <f t="shared" ref="C24" si="5">DEC2HEX(B24 + _xlfn.BITLSHIFT(B$22,8),4)</f>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="221" t="str">
+        <f t="shared" ref="E26:E40" si="8">DEC2HEX(D26 + _xlfn.BITLSHIFT(D$24,8),4)</f>
         <v>0201</v>
       </c>
-      <c r="I24" s="1">
-        <f>G24*H24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="217" t="s">
-        <v>272</v>
-      </c>
-      <c r="B31" s="218">
+      <c r="F26" s="224" t="s">
+        <v>292</v>
+      </c>
+      <c r="G26" s="258">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1">
+        <f>I26*J26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0202</v>
+      </c>
+      <c r="F27" s="224" t="s">
+        <v>293</v>
+      </c>
+      <c r="G27" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D28">
         <v>3</v>
       </c>
-      <c r="C31" s="220"/>
-      <c r="D31" s="223"/>
-      <c r="E31" s="265"/>
-      <c r="I31" s="218">
-        <f>SUM(I32:I33)</f>
-        <v>0</v>
+      <c r="E28" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0203</v>
+      </c>
+      <c r="F28" s="224" t="s">
+        <v>294</v>
+      </c>
+      <c r="G28" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0204</v>
+      </c>
+      <c r="F29" s="224" t="s">
+        <v>291</v>
+      </c>
+      <c r="G29" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0205</v>
+      </c>
+      <c r="F30" s="224" t="s">
+        <v>296</v>
+      </c>
+      <c r="G30" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0206</v>
+      </c>
+      <c r="F31" s="224" t="s">
+        <v>297</v>
+      </c>
+      <c r="G31" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0207</v>
+      </c>
+      <c r="F32" s="224" t="s">
+        <v>298</v>
+      </c>
+      <c r="G32" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0208</v>
+      </c>
+      <c r="F33" s="224" t="s">
+        <v>295</v>
+      </c>
+      <c r="G33" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>9</v>
+      </c>
+      <c r="E34" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>0209</v>
+      </c>
+      <c r="F34" s="224" t="s">
+        <v>299</v>
+      </c>
+      <c r="G34" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>020A</v>
+      </c>
+      <c r="F35" s="224" t="s">
+        <v>300</v>
+      </c>
+      <c r="G35" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>11</v>
+      </c>
+      <c r="E36" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>020B</v>
+      </c>
+      <c r="F36" s="224" t="s">
+        <v>301</v>
+      </c>
+      <c r="G36" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>12</v>
+      </c>
+      <c r="E37" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>020C</v>
+      </c>
+      <c r="F37" s="224" t="s">
+        <v>302</v>
+      </c>
+      <c r="G37" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>13</v>
+      </c>
+      <c r="E38" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>020D</v>
+      </c>
+      <c r="F38" s="224" t="s">
+        <v>303</v>
+      </c>
+      <c r="G38" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>14</v>
+      </c>
+      <c r="E39" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>020E</v>
+      </c>
+      <c r="F39" s="224" t="s">
+        <v>304</v>
+      </c>
+      <c r="G39" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>15</v>
+      </c>
+      <c r="E40" s="221" t="str">
+        <f t="shared" si="8"/>
+        <v>020F</v>
+      </c>
+      <c r="F40" s="224" t="s">
+        <v>305</v>
+      </c>
+      <c r="G40" s="258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="218" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41" s="218" t="s">
+        <v>270</v>
+      </c>
+      <c r="C41" s="218" t="s">
+        <v>281</v>
+      </c>
+      <c r="D41" s="218">
+        <v>3</v>
+      </c>
+      <c r="E41" s="220"/>
+      <c r="F41" s="223"/>
+      <c r="G41" s="265"/>
+      <c r="K41" s="218">
+        <f>SUM(K42:K43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="221" t="str">
+        <f>DEC2HEX(D42 + _xlfn.BITLSHIFT(D$41,8),4)</f>
+        <v>0300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="221" t="str">
+        <f>DEC2HEX(D43 + _xlfn.BITLSHIFT(D$41,8),4)</f>
+        <v>0301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created GarageDoorControllerProd building process + updated arch
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43786FC-560D-4A6F-9FBD-476EFE6C09C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CDEC63-4528-420D-86B4-102E404C62A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
   <sheets>
     <sheet name="frames-data-bits" sheetId="2" r:id="rId1"/>
@@ -4940,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D135A44-A127-4252-B653-8392D6AD3A28}">
   <dimension ref="A2:BO45"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5764,41 +5764,41 @@
       <c r="G8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="238" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="M8" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="N8" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="O8" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="184" t="s">
-        <v>46</v>
-      </c>
-      <c r="M8" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="N8" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="P8" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q8" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="R8" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="186" t="s">
-        <v>46</v>
+      <c r="P8" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="S8" s="44" t="s">
+        <v>42</v>
       </c>
       <c r="T8" s="184" t="s">
         <v>46</v>
@@ -9135,7 +9135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36880ADF-04C9-4A12-8EFC-224812D037A0}">
   <dimension ref="A3:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated debug script, refactored attributes, added preprocessor
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5C78FA-48A2-4AE6-83D9-8DBFE0848B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633C9153-8273-4607-A810-FF08B9C724FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
   <sheets>
     <sheet name="frames-data-bits" sheetId="2" r:id="rId1"/>
@@ -13338,8 +13338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
   <dimension ref="A1:V381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added support for custom board + refactoring
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633C9153-8273-4607-A810-FF08B9C724FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECBD3BE-C8AE-4BAE-A4E2-E4384B3FB08A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
   <sheets>
     <sheet name="frames-data-bits" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="352">
   <si>
     <t>temperature</t>
   </si>
@@ -831,15 +831,9 @@
     <t>CR</t>
   </si>
   <si>
-    <t>GarageDoorController</t>
-  </si>
-  <si>
     <t>Device used</t>
   </si>
   <si>
-    <t>OutdoorSensor1</t>
-  </si>
-  <si>
     <t>SCHEDULE</t>
   </si>
   <si>
@@ -1081,13 +1075,34 @@
   </si>
   <si>
     <t>calculated_abstime</t>
+  </si>
+  <si>
+    <t>events.total</t>
+  </si>
+  <si>
+    <t>last_event_error</t>
+  </si>
+  <si>
+    <t>GarageDoorControllerDev</t>
+  </si>
+  <si>
+    <t>GarageDoorControllerProd</t>
+  </si>
+  <si>
+    <t>GarageDoorControllerProdPCB</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>TempSensDev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,6 +1205,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1602,7 +1626,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="277">
+  <cellXfs count="282">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2300,6 +2324,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2800,7 +2829,7 @@
   <dimension ref="B1:AH59"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13:U13"/>
+      <selection activeCell="W53" sqref="W53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3145,28 +3174,28 @@
         <v>81</v>
       </c>
       <c r="N13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="R13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="S13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="T13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="U13" s="167" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="V13" s="25" t="s">
         <v>45</v>
@@ -3958,7 +3987,7 @@
         <v>153</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -4524,7 +4553,7 @@
         <v>152</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
@@ -4537,7 +4566,7 @@
       <c r="L40" s="48"/>
       <c r="M40" s="48"/>
       <c r="T40" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="2:34" x14ac:dyDescent="0.2">
@@ -4567,7 +4596,7 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>144</v>
@@ -5090,7 +5119,7 @@
     </row>
     <row r="52" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>15</v>
@@ -5215,16 +5244,16 @@
     </row>
     <row r="55" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C55" s="268" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D55" s="268" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E55" s="268" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F55" s="268" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G55" s="269" t="s">
         <v>252</v>
@@ -5251,24 +5280,24 @@
         <v>252</v>
       </c>
       <c r="O55" s="270" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P55" s="270" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q55" s="270" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="R55" s="270" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="57" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C57" s="268" t="s">
+        <v>317</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="58" spans="2:34" x14ac:dyDescent="0.2">
@@ -5276,15 +5305,15 @@
         <v>252</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C59" s="270" t="s">
+        <v>318</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -5299,8 +5328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D135A44-A127-4252-B653-8392D6AD3A28}">
   <dimension ref="A2:BO45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6655,23 +6684,23 @@
       <c r="S12" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="T12" s="187" t="s">
-        <v>250</v>
-      </c>
-      <c r="U12" s="188" t="s">
-        <v>250</v>
-      </c>
-      <c r="V12" s="188" t="s">
-        <v>250</v>
-      </c>
-      <c r="W12" s="188" t="s">
-        <v>250</v>
-      </c>
-      <c r="X12" s="188" t="s">
-        <v>250</v>
-      </c>
-      <c r="Y12" s="188" t="s">
-        <v>250</v>
+      <c r="T12" s="184" t="s">
+        <v>46</v>
+      </c>
+      <c r="U12" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="V12" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="W12" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="X12" s="185" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y12" s="185" t="s">
+        <v>46</v>
       </c>
       <c r="Z12" s="188" t="s">
         <v>250</v>
@@ -6685,23 +6714,23 @@
       <c r="AC12" s="188" t="s">
         <v>250</v>
       </c>
-      <c r="AD12" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE12" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF12" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG12" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH12" s="185" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI12" s="186" t="s">
-        <v>46</v>
+      <c r="AD12" s="188" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE12" s="188" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF12" s="188" t="s">
+        <v>250</v>
+      </c>
+      <c r="AG12" s="188" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH12" s="188" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI12" s="238" t="s">
+        <v>250</v>
       </c>
       <c r="AJ12" s="184" t="s">
         <v>46</v>
@@ -9492,10 +9521,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36880ADF-04C9-4A12-8EFC-224812D037A0}">
-  <dimension ref="A3:K93"/>
+  <dimension ref="A3:M93"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P58" sqref="P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9505,7 +9534,9 @@
     <col min="6" max="6" width="5.140625" style="67" customWidth="1"/>
     <col min="8" max="8" width="18" style="90" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="66"/>
-    <col min="11" max="11" width="21.140625" style="67" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="67" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -9565,7 +9596,7 @@
         <v>8</v>
       </c>
       <c r="K4" s="256" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9729,7 +9760,7 @@
         <v>45</v>
       </c>
       <c r="K11" s="256" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9820,7 +9851,7 @@
       <c r="I16" s="63"/>
       <c r="K16" s="63"/>
     </row>
-    <row r="17" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>54</v>
       </c>
@@ -9848,7 +9879,7 @@
       <c r="I17" s="65"/>
       <c r="K17" s="256"/>
     </row>
-    <row r="18" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
         <v>56</v>
       </c>
@@ -9878,7 +9909,7 @@
       <c r="I18" s="65"/>
       <c r="K18" s="256"/>
     </row>
-    <row r="19" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="55" t="s">
         <v>59</v>
       </c>
@@ -9906,7 +9937,7 @@
       <c r="I19" s="65"/>
       <c r="K19" s="256"/>
     </row>
-    <row r="20" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="50"/>
       <c r="C20" s="50"/>
       <c r="D20" s="82">
@@ -9929,7 +9960,7 @@
       <c r="I20" s="65"/>
       <c r="K20" s="256"/>
     </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>55</v>
       </c>
@@ -9956,10 +9987,16 @@
         <v>248</v>
       </c>
       <c r="K23" s="257" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="L23" s="278" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="279" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="54" t="s">
         <v>54</v>
       </c>
@@ -9986,8 +10023,14 @@
       </c>
       <c r="I24" s="65"/>
       <c r="K24" s="258"/>
-    </row>
-    <row r="25" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L24" s="35">
+        <v>0</v>
+      </c>
+      <c r="M24" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
         <v>56</v>
       </c>
@@ -10018,8 +10061,14 @@
         <v>256</v>
       </c>
       <c r="K25" s="258"/>
-    </row>
-    <row r="26" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="35">
+        <v>0</v>
+      </c>
+      <c r="M25" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="55" t="s">
         <v>59</v>
       </c>
@@ -10046,8 +10095,14 @@
         <v>256</v>
       </c>
       <c r="K26" s="258"/>
-    </row>
-    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="35">
+        <v>0</v>
+      </c>
+      <c r="M26" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
       <c r="D27" s="77">
@@ -10069,8 +10124,14 @@
         <v>256</v>
       </c>
       <c r="K27" s="258"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="35">
+        <v>0</v>
+      </c>
+      <c r="M27" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D28" s="77">
         <v>4</v>
       </c>
@@ -10090,8 +10151,14 @@
         <v>256</v>
       </c>
       <c r="K28" s="259"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="35">
+        <v>0</v>
+      </c>
+      <c r="M28" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D29" s="77">
         <v>5</v>
       </c>
@@ -10111,8 +10178,14 @@
         <v>256</v>
       </c>
       <c r="K29" s="259"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="35">
+        <v>0</v>
+      </c>
+      <c r="M29" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D30" s="77">
         <v>6</v>
       </c>
@@ -10132,8 +10205,14 @@
         <v>256</v>
       </c>
       <c r="K30" s="259"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="35">
+        <v>0</v>
+      </c>
+      <c r="M30" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D31" s="77">
         <v>7</v>
       </c>
@@ -10153,8 +10232,14 @@
         <v>256</v>
       </c>
       <c r="K31" s="259"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="35">
+        <v>0</v>
+      </c>
+      <c r="M31" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" s="77">
         <v>8</v>
       </c>
@@ -10173,11 +10258,15 @@
       <c r="I32" s="249" t="s">
         <v>262</v>
       </c>
-      <c r="K32" s="259" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="259"/>
+      <c r="L32" s="277">
+        <v>1</v>
+      </c>
+      <c r="M32" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D33" s="77">
         <v>9</v>
       </c>
@@ -10197,8 +10286,14 @@
         <v>262</v>
       </c>
       <c r="K33" s="259"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="277">
+        <v>1</v>
+      </c>
+      <c r="M33" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D34" s="77">
         <v>10</v>
       </c>
@@ -10218,8 +10313,14 @@
         <v>262</v>
       </c>
       <c r="K34" s="259"/>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="277">
+        <v>1</v>
+      </c>
+      <c r="M34" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D35" s="77">
         <v>11</v>
       </c>
@@ -10239,8 +10340,14 @@
         <v>262</v>
       </c>
       <c r="K35" s="259"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="277">
+        <v>1</v>
+      </c>
+      <c r="M35" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D36" s="77">
         <v>12</v>
       </c>
@@ -10260,8 +10367,14 @@
         <v>262</v>
       </c>
       <c r="K36" s="259"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="277">
+        <v>1</v>
+      </c>
+      <c r="M36" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D37" s="77">
         <v>13</v>
       </c>
@@ -10281,8 +10394,14 @@
         <v>262</v>
       </c>
       <c r="K37" s="259"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="277">
+        <v>1</v>
+      </c>
+      <c r="M37" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D38" s="77">
         <v>14</v>
       </c>
@@ -10302,8 +10421,14 @@
         <v>262</v>
       </c>
       <c r="K38" s="259"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="277">
+        <v>1</v>
+      </c>
+      <c r="M38" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D39" s="77">
         <v>15</v>
       </c>
@@ -10323,8 +10448,14 @@
         <v>262</v>
       </c>
       <c r="K39" s="259"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="277">
+        <v>1</v>
+      </c>
+      <c r="M39" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D40" s="77">
         <v>16</v>
       </c>
@@ -10343,8 +10474,14 @@
         <v>257</v>
       </c>
       <c r="K40" s="259"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="277">
+        <v>2</v>
+      </c>
+      <c r="M40" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D41" s="77">
         <v>17</v>
       </c>
@@ -10363,8 +10500,14 @@
         <v>257</v>
       </c>
       <c r="K41" s="259"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="277">
+        <v>2</v>
+      </c>
+      <c r="M41" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D42" s="77">
         <v>18</v>
       </c>
@@ -10383,8 +10526,14 @@
         <v>257</v>
       </c>
       <c r="K42" s="259"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="277">
+        <v>2</v>
+      </c>
+      <c r="M42" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D43" s="77">
         <v>19</v>
       </c>
@@ -10403,8 +10552,14 @@
         <v>257</v>
       </c>
       <c r="K43" s="259"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="277">
+        <v>2</v>
+      </c>
+      <c r="M43" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D44" s="77">
         <v>20</v>
       </c>
@@ -10423,8 +10578,14 @@
         <v>257</v>
       </c>
       <c r="K44" s="259"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="277">
+        <v>2</v>
+      </c>
+      <c r="M44" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D45" s="77">
         <v>21</v>
       </c>
@@ -10443,8 +10604,14 @@
         <v>257</v>
       </c>
       <c r="K45" s="259"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="277">
+        <v>2</v>
+      </c>
+      <c r="M45" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D46" s="77">
         <v>22</v>
       </c>
@@ -10463,8 +10630,14 @@
         <v>257</v>
       </c>
       <c r="K46" s="259"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="277">
+        <v>2</v>
+      </c>
+      <c r="M46" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D47" s="77">
         <v>23</v>
       </c>
@@ -10483,8 +10656,14 @@
         <v>257</v>
       </c>
       <c r="K47" s="259"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="277">
+        <v>2</v>
+      </c>
+      <c r="M47" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D48" s="77">
         <v>24</v>
       </c>
@@ -10503,10 +10682,16 @@
         <v>258</v>
       </c>
       <c r="K48" s="259" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+      <c r="L48" s="277">
+        <v>3</v>
+      </c>
+      <c r="M48" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D49" s="77">
         <v>25</v>
       </c>
@@ -10524,9 +10709,17 @@
       <c r="I49" s="249" t="s">
         <v>258</v>
       </c>
-      <c r="K49" s="259"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="259" t="s">
+        <v>348</v>
+      </c>
+      <c r="L49" s="277">
+        <v>3</v>
+      </c>
+      <c r="M49" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D50" s="77">
         <v>26</v>
       </c>
@@ -10544,9 +10737,17 @@
       <c r="I50" s="249" t="s">
         <v>258</v>
       </c>
-      <c r="K50" s="259"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="259" t="s">
+        <v>351</v>
+      </c>
+      <c r="L50" s="277">
+        <v>3</v>
+      </c>
+      <c r="M50" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D51" s="77">
         <v>27</v>
       </c>
@@ -10565,8 +10766,14 @@
         <v>258</v>
       </c>
       <c r="K51" s="259"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="277">
+        <v>3</v>
+      </c>
+      <c r="M51" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D52" s="77">
         <v>28</v>
       </c>
@@ -10585,8 +10792,14 @@
         <v>258</v>
       </c>
       <c r="K52" s="259"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="277">
+        <v>3</v>
+      </c>
+      <c r="M52" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D53" s="77">
         <v>29</v>
       </c>
@@ -10605,8 +10818,14 @@
         <v>258</v>
       </c>
       <c r="K53" s="259"/>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="277">
+        <v>3</v>
+      </c>
+      <c r="M53" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D54" s="77">
         <v>30</v>
       </c>
@@ -10625,8 +10844,14 @@
         <v>258</v>
       </c>
       <c r="K54" s="259"/>
-    </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="277">
+        <v>3</v>
+      </c>
+      <c r="M54" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D55" s="77">
         <v>31</v>
       </c>
@@ -10645,8 +10870,14 @@
         <v>258</v>
       </c>
       <c r="K55" s="259"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="277">
+        <v>3</v>
+      </c>
+      <c r="M55" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D56" s="77">
         <v>32</v>
       </c>
@@ -10665,8 +10896,14 @@
         <v>259</v>
       </c>
       <c r="K56" s="259"/>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="277">
+        <v>4</v>
+      </c>
+      <c r="M56" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D57" s="77">
         <v>33</v>
       </c>
@@ -10685,8 +10922,14 @@
         <v>259</v>
       </c>
       <c r="K57" s="259"/>
-    </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="277">
+        <v>4</v>
+      </c>
+      <c r="M57" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D58" s="77">
         <v>34</v>
       </c>
@@ -10705,8 +10948,14 @@
         <v>259</v>
       </c>
       <c r="K58" s="259"/>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="277">
+        <v>4</v>
+      </c>
+      <c r="M58" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D59" s="77">
         <v>35</v>
       </c>
@@ -10725,8 +10974,14 @@
         <v>259</v>
       </c>
       <c r="K59" s="259"/>
-    </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="277">
+        <v>4</v>
+      </c>
+      <c r="M59" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D60" s="77">
         <v>36</v>
       </c>
@@ -10745,8 +11000,14 @@
         <v>259</v>
       </c>
       <c r="K60" s="259"/>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="277">
+        <v>4</v>
+      </c>
+      <c r="M60" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D61" s="77">
         <v>37</v>
       </c>
@@ -10765,8 +11026,14 @@
         <v>259</v>
       </c>
       <c r="K61" s="259"/>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="277">
+        <v>4</v>
+      </c>
+      <c r="M61" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D62" s="77">
         <v>38</v>
       </c>
@@ -10785,8 +11052,14 @@
         <v>259</v>
       </c>
       <c r="K62" s="259"/>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="277">
+        <v>4</v>
+      </c>
+      <c r="M62" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D63" s="77">
         <v>39</v>
       </c>
@@ -10805,8 +11078,14 @@
         <v>259</v>
       </c>
       <c r="K63" s="259"/>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="277">
+        <v>4</v>
+      </c>
+      <c r="M63" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D64" s="77">
         <v>40</v>
       </c>
@@ -10824,9 +11103,17 @@
       <c r="I64" s="249" t="s">
         <v>260</v>
       </c>
-      <c r="K64" s="259"/>
-    </row>
-    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="258" t="s">
+        <v>349</v>
+      </c>
+      <c r="L64" s="277">
+        <v>5</v>
+      </c>
+      <c r="M64" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D65" s="77">
         <v>41</v>
       </c>
@@ -10845,8 +11132,14 @@
         <v>260</v>
       </c>
       <c r="K65" s="259"/>
-    </row>
-    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L65" s="277">
+        <v>5</v>
+      </c>
+      <c r="M65" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D66" s="77">
         <v>42</v>
       </c>
@@ -10865,8 +11158,14 @@
         <v>260</v>
       </c>
       <c r="K66" s="259"/>
-    </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L66" s="277">
+        <v>5</v>
+      </c>
+      <c r="M66" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D67" s="77">
         <v>43</v>
       </c>
@@ -10885,8 +11184,14 @@
         <v>260</v>
       </c>
       <c r="K67" s="259"/>
-    </row>
-    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L67" s="277">
+        <v>5</v>
+      </c>
+      <c r="M67" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D68" s="77">
         <v>44</v>
       </c>
@@ -10905,8 +11210,14 @@
         <v>260</v>
       </c>
       <c r="K68" s="259"/>
-    </row>
-    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L68" s="277">
+        <v>5</v>
+      </c>
+      <c r="M68" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D69" s="77">
         <v>45</v>
       </c>
@@ -10925,8 +11236,14 @@
         <v>260</v>
       </c>
       <c r="K69" s="259"/>
-    </row>
-    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L69" s="277">
+        <v>5</v>
+      </c>
+      <c r="M69" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D70" s="77">
         <v>46</v>
       </c>
@@ -10945,8 +11262,14 @@
         <v>260</v>
       </c>
       <c r="K70" s="259"/>
-    </row>
-    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L70" s="277">
+        <v>5</v>
+      </c>
+      <c r="M70" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D71" s="77">
         <v>47</v>
       </c>
@@ -10965,8 +11288,14 @@
         <v>260</v>
       </c>
       <c r="K71" s="259"/>
-    </row>
-    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L71" s="277">
+        <v>5</v>
+      </c>
+      <c r="M71" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D72" s="77">
         <v>48</v>
       </c>
@@ -10985,8 +11314,14 @@
         <v>261</v>
       </c>
       <c r="K72" s="259"/>
-    </row>
-    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L72" s="277">
+        <v>6</v>
+      </c>
+      <c r="M72" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D73" s="77">
         <v>49</v>
       </c>
@@ -11005,8 +11340,14 @@
         <v>261</v>
       </c>
       <c r="K73" s="259"/>
-    </row>
-    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L73" s="277">
+        <v>6</v>
+      </c>
+      <c r="M73" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D74" s="77">
         <v>50</v>
       </c>
@@ -11025,8 +11366,14 @@
         <v>261</v>
       </c>
       <c r="K74" s="259"/>
-    </row>
-    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L74" s="277">
+        <v>6</v>
+      </c>
+      <c r="M74" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D75" s="77">
         <v>51</v>
       </c>
@@ -11045,8 +11392,14 @@
         <v>261</v>
       </c>
       <c r="K75" s="259"/>
-    </row>
-    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L75" s="277">
+        <v>6</v>
+      </c>
+      <c r="M75" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D76" s="77">
         <v>52</v>
       </c>
@@ -11065,8 +11418,14 @@
         <v>261</v>
       </c>
       <c r="K76" s="259"/>
-    </row>
-    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L76" s="277">
+        <v>6</v>
+      </c>
+      <c r="M76" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D77" s="77">
         <v>53</v>
       </c>
@@ -11085,8 +11444,14 @@
         <v>261</v>
       </c>
       <c r="K77" s="259"/>
-    </row>
-    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L77" s="277">
+        <v>6</v>
+      </c>
+      <c r="M77" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D78" s="77">
         <v>54</v>
       </c>
@@ -11105,8 +11470,14 @@
         <v>261</v>
       </c>
       <c r="K78" s="259"/>
-    </row>
-    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L78" s="277">
+        <v>6</v>
+      </c>
+      <c r="M78" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D79" s="77">
         <v>55</v>
       </c>
@@ -11125,8 +11496,14 @@
         <v>261</v>
       </c>
       <c r="K79" s="259"/>
-    </row>
-    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L79" s="277">
+        <v>6</v>
+      </c>
+      <c r="M79" s="280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D80" s="77">
         <v>56</v>
       </c>
@@ -11145,8 +11522,14 @@
         <v>46</v>
       </c>
       <c r="K80" s="259"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" s="277">
+        <v>7</v>
+      </c>
+      <c r="M80" s="280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D81" s="77">
         <v>57</v>
       </c>
@@ -11165,8 +11548,14 @@
         <v>46</v>
       </c>
       <c r="K81" s="259"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" s="277">
+        <v>7</v>
+      </c>
+      <c r="M81" s="280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D82" s="77">
         <v>58</v>
       </c>
@@ -11185,8 +11574,14 @@
         <v>46</v>
       </c>
       <c r="K82" s="259"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" s="277">
+        <v>7</v>
+      </c>
+      <c r="M82" s="280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D83" s="77">
         <v>59</v>
       </c>
@@ -11205,8 +11600,14 @@
         <v>46</v>
       </c>
       <c r="K83" s="259"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" s="277">
+        <v>7</v>
+      </c>
+      <c r="M83" s="280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D84" s="77">
         <v>60</v>
       </c>
@@ -11225,8 +11626,14 @@
         <v>46</v>
       </c>
       <c r="K84" s="259"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" s="277">
+        <v>7</v>
+      </c>
+      <c r="M84" s="280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D85" s="77">
         <v>61</v>
       </c>
@@ -11245,8 +11652,14 @@
         <v>46</v>
       </c>
       <c r="K85" s="259"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" s="277">
+        <v>7</v>
+      </c>
+      <c r="M85" s="280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D86" s="77">
         <v>62</v>
       </c>
@@ -11268,8 +11681,14 @@
         <v>46</v>
       </c>
       <c r="K86" s="259"/>
-    </row>
-    <row r="87" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L86" s="277">
+        <v>7</v>
+      </c>
+      <c r="M86" s="280">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D87" s="253">
         <v>63</v>
       </c>
@@ -11289,13 +11708,19 @@
       </c>
       <c r="I87" s="252"/>
       <c r="K87" s="260"/>
-    </row>
-    <row r="89" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L87" s="56">
+        <v>7</v>
+      </c>
+      <c r="M87" s="281">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B89" s="59" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C89" s="60"/>
       <c r="D89" s="63" t="s">
@@ -11318,12 +11743,12 @@
       </c>
       <c r="K89" s="63"/>
     </row>
-    <row r="90" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="54" t="s">
         <v>54</v>
       </c>
       <c r="B90" s="271" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C90" s="52"/>
       <c r="D90" s="272">
@@ -11342,7 +11767,7 @@
       <c r="I90" s="65"/>
       <c r="K90" s="256"/>
     </row>
-    <row r="91" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="54" t="s">
         <v>56</v>
       </c>
@@ -11368,7 +11793,7 @@
       <c r="I91" s="65"/>
       <c r="K91" s="256"/>
     </row>
-    <row r="92" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="55" t="s">
         <v>59</v>
       </c>
@@ -11391,15 +11816,15 @@
       <c r="I92" s="65"/>
       <c r="K92" s="256"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D93" s="67" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E93" s="67" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F93" s="67" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -11693,28 +12118,28 @@
         <v>81</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="R8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="S8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="T8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="U8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="V8" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="W8" s="25" t="s">
         <v>45</v>
@@ -12618,7 +13043,7 @@
       <c r="S4" s="94"/>
       <c r="T4" s="95"/>
       <c r="V4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -12673,12 +13098,12 @@
         <v>126</v>
       </c>
       <c r="V5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="V6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -13217,7 +13642,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="212" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C16" s="96">
         <v>0</v>
@@ -13256,7 +13681,7 @@
         <v>104</v>
       </c>
       <c r="P16" s="262" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Q16" s="262" t="s">
         <v>115</v>
@@ -13336,10 +13761,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
-  <dimension ref="A1:V381"/>
+  <dimension ref="A1:V383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13376,7 +13801,7 @@
         <v>157</v>
       </c>
       <c r="G1" s="63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>161</v>
@@ -13406,7 +13831,7 @@
         <v>173</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="218" customFormat="1" x14ac:dyDescent="0.25">
@@ -13414,7 +13839,7 @@
         <v>160</v>
       </c>
       <c r="C2" s="218" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D2" s="218">
         <v>0</v>
@@ -13426,13 +13851,13 @@
         <v>35</v>
       </c>
       <c r="K2" s="263" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="L2" s="263" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="M2" s="263" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="N2" s="263" t="s">
         <v>88</v>
@@ -13541,7 +13966,7 @@
         <v>0020</v>
       </c>
       <c r="F5" s="266" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G5" s="34">
         <v>32</v>
@@ -13573,7 +13998,7 @@
         <v>0021</v>
       </c>
       <c r="F6" s="266" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
@@ -13589,7 +14014,7 @@
         <v>0022</v>
       </c>
       <c r="F7" s="266" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -13605,7 +14030,7 @@
         <v>0023</v>
       </c>
       <c r="F8" s="266" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
@@ -13621,7 +14046,7 @@
         <v>0024</v>
       </c>
       <c r="F9" s="266" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -13637,7 +14062,7 @@
         <v>0025</v>
       </c>
       <c r="F10" s="266" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -13653,7 +14078,7 @@
         <v>0026</v>
       </c>
       <c r="F11" s="266" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -13669,7 +14094,7 @@
         <v>0027</v>
       </c>
       <c r="F12" s="266" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
@@ -13704,7 +14129,7 @@
         <v>159</v>
       </c>
       <c r="C15" s="218" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D15" s="218">
         <v>1</v>
@@ -13712,8 +14137,8 @@
       <c r="E15" s="220"/>
       <c r="F15" s="265"/>
       <c r="G15" s="218">
-        <f>SUM(G16:G34)</f>
-        <v>59</v>
+        <f>SUM(G16:G36)</f>
+        <v>65</v>
       </c>
       <c r="K15" s="263"/>
       <c r="L15" s="263"/>
@@ -13765,17 +14190,17 @@
         <v>1</v>
       </c>
       <c r="E17" s="221" t="str">
-        <f t="shared" ref="E17:E33" si="2">DEC2HEX(_xlfn.BITLSHIFT(D17,4) + _xlfn.BITLSHIFT(D$15,12),4)</f>
+        <f t="shared" ref="E17:E35" si="2">DEC2HEX(_xlfn.BITLSHIFT(D17,4) + _xlfn.BITLSHIFT(D$15,12),4)</f>
         <v>1010</v>
       </c>
       <c r="F17" s="266" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G17" s="34">
         <v>4</v>
       </c>
       <c r="H17" s="34">
-        <f t="shared" ref="H17:H32" si="3">ROUNDUP(G17/4,0)</f>
+        <f t="shared" ref="H17:H34" si="3">ROUNDUP(G17/4,0)</f>
         <v>1</v>
       </c>
       <c r="I17" t="s">
@@ -13807,7 +14232,7 @@
         <v>1020</v>
       </c>
       <c r="F18" s="266" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G18" s="34">
         <v>4</v>
@@ -13829,7 +14254,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="267" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="4:22" x14ac:dyDescent="0.25">
@@ -13841,7 +14266,7 @@
         <v>1030</v>
       </c>
       <c r="F19" s="266" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G19" s="34">
         <v>4</v>
@@ -13864,7 +14289,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="267" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O19" s="264"/>
     </row>
@@ -13877,7 +14302,7 @@
         <v>1040</v>
       </c>
       <c r="F20" s="266" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G20" s="34">
         <v>4</v>
@@ -13912,7 +14337,7 @@
         <v>1050</v>
       </c>
       <c r="F21" s="266" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G21" s="34">
         <v>4</v>
@@ -13947,7 +14372,7 @@
         <v>1060</v>
       </c>
       <c r="F22" s="266" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G22" s="34">
         <v>4</v>
@@ -13982,7 +14407,7 @@
         <v>1070</v>
       </c>
       <c r="F23" s="266" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G23" s="34">
         <v>4</v>
@@ -14017,7 +14442,7 @@
         <v>1080</v>
       </c>
       <c r="F24" s="266" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G24" s="34">
         <v>4</v>
@@ -14052,7 +14477,7 @@
         <v>1090</v>
       </c>
       <c r="F25" s="266" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G25" s="34">
         <v>4</v>
@@ -14087,7 +14512,7 @@
         <v>10A0</v>
       </c>
       <c r="F26" s="266" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G26" s="34">
         <v>4</v>
@@ -14122,7 +14547,7 @@
         <v>10B0</v>
       </c>
       <c r="F27" s="266" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G27" s="34">
         <v>4</v>
@@ -14157,7 +14582,7 @@
         <v>10C0</v>
       </c>
       <c r="F28" s="266" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G28" s="34">
         <v>4</v>
@@ -14195,7 +14620,7 @@
         <v>246</v>
       </c>
       <c r="V28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="4:22" x14ac:dyDescent="0.25">
@@ -14207,7 +14632,7 @@
         <v>10D0</v>
       </c>
       <c r="F29" s="266" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G29" s="34">
         <v>4</v>
@@ -14242,17 +14667,17 @@
         <v>10E0</v>
       </c>
       <c r="F30" s="266" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="G30" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H30" s="34">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="66">
@@ -14277,7 +14702,7 @@
         <v>10F0</v>
       </c>
       <c r="F31" s="266" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G31" s="34">
         <v>1</v>
@@ -14312,7 +14737,7 @@
         <v>1100</v>
       </c>
       <c r="F32" s="266" t="s">
-        <v>177</v>
+        <v>332</v>
       </c>
       <c r="G32" s="34">
         <v>1</v>
@@ -14346,154 +14771,204 @@
         <f t="shared" si="2"/>
         <v>1110</v>
       </c>
-      <c r="F33" s="266"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
+      <c r="F33" s="266" t="s">
+        <v>346</v>
+      </c>
+      <c r="G33" s="34">
+        <v>2</v>
+      </c>
+      <c r="H33" s="34">
+        <f t="shared" ref="H33" si="4">ROUNDUP(G33/4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>178</v>
+      </c>
       <c r="J33" s="1"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="65"/>
+      <c r="K33" s="66">
+        <v>1</v>
+      </c>
+      <c r="L33" s="66">
+        <v>0</v>
+      </c>
+      <c r="M33" s="66">
+        <v>0</v>
+      </c>
+      <c r="N33" s="65">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F34" s="266"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="D34">
+        <v>18</v>
+      </c>
+      <c r="E34" s="221" t="str">
+        <f t="shared" si="2"/>
+        <v>1120</v>
+      </c>
+      <c r="F34" s="266" t="s">
+        <v>177</v>
+      </c>
+      <c r="G34" s="34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="34">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>178</v>
+      </c>
       <c r="J34" s="1"/>
-      <c r="K34" s="66"/>
-      <c r="L34" s="66"/>
-      <c r="M34" s="66"/>
-      <c r="N34" s="65"/>
+      <c r="K34" s="66">
+        <v>1</v>
+      </c>
+      <c r="L34" s="66">
+        <v>0</v>
+      </c>
+      <c r="M34" s="66">
+        <v>0</v>
+      </c>
+      <c r="N34" s="65">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>19</v>
+      </c>
+      <c r="E35" s="221" t="str">
+        <f t="shared" si="2"/>
+        <v>1130</v>
+      </c>
       <c r="F35" s="266"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
       <c r="J35" s="1"/>
       <c r="K35" s="66"/>
       <c r="L35" s="66"/>
       <c r="M35" s="66"/>
       <c r="N35" s="65"/>
     </row>
-    <row r="36" spans="1:21" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="217" t="s">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F36" s="266"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="66"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="66"/>
+      <c r="N36" s="65"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F37" s="266"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="65"/>
+    </row>
+    <row r="38" spans="1:21" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="217" t="s">
+        <v>277</v>
+      </c>
+      <c r="C38" s="218" t="s">
+        <v>275</v>
+      </c>
+      <c r="D38" s="218">
+        <v>2</v>
+      </c>
+      <c r="E38" s="220"/>
+      <c r="F38" s="265"/>
+      <c r="G38" s="218">
+        <f>SUM(G39:G44)</f>
+        <v>8</v>
+      </c>
+      <c r="K38" s="263"/>
+      <c r="L38" s="263"/>
+      <c r="M38" s="263"/>
+      <c r="N38" s="263"/>
+      <c r="O38" s="263"/>
+      <c r="P38" s="276"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" s="221" t="str">
+        <f>DEC2HEX(_xlfn.BITLSHIFT(D39,4) + _xlfn.BITLSHIFT(D$38,12),4)</f>
+        <v>2000</v>
+      </c>
+      <c r="F39" s="266" t="s">
+        <v>265</v>
+      </c>
+      <c r="G39" s="34">
+        <v>4</v>
+      </c>
+      <c r="H39" s="34">
+        <f>ROUNDUP(G39/4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>175</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="66">
+        <v>0</v>
+      </c>
+      <c r="L39" s="66">
+        <v>1</v>
+      </c>
+      <c r="M39" s="66">
+        <v>0</v>
+      </c>
+      <c r="N39" s="65">
+        <v>1</v>
+      </c>
+      <c r="R39" t="s">
+        <v>278</v>
+      </c>
+      <c r="S39" t="s">
         <v>279</v>
       </c>
-      <c r="C36" s="218" t="s">
-        <v>277</v>
-      </c>
-      <c r="D36" s="218">
-        <v>2</v>
-      </c>
-      <c r="E36" s="220"/>
-      <c r="F36" s="265"/>
-      <c r="G36" s="218">
-        <f>SUM(G37:G42)</f>
-        <v>8</v>
-      </c>
-      <c r="K36" s="263"/>
-      <c r="L36" s="263"/>
-      <c r="M36" s="263"/>
-      <c r="N36" s="263"/>
-      <c r="O36" s="263"/>
-      <c r="P36" s="276"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37" s="221" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(D37,4) + _xlfn.BITLSHIFT(D$36,12),4)</f>
-        <v>2000</v>
-      </c>
-      <c r="F37" s="266" t="s">
-        <v>267</v>
-      </c>
-      <c r="G37" s="34">
+      <c r="T39">
+        <v>10</v>
+      </c>
+      <c r="U39" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="221" t="str">
+        <f>DEC2HEX(_xlfn.BITLSHIFT(D40,4) + _xlfn.BITLSHIFT(D$38,12),4)</f>
+        <v>2010</v>
+      </c>
+      <c r="F40" s="266" t="s">
+        <v>342</v>
+      </c>
+      <c r="G40" s="34">
         <v>4</v>
       </c>
-      <c r="H37" s="34">
-        <f>ROUNDUP(G37/4,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="H40" s="34">
+        <f>ROUNDUP(G40/4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
         <v>175</v>
       </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="66">
-        <v>0</v>
-      </c>
-      <c r="L37" s="66">
-        <v>1</v>
-      </c>
-      <c r="M37" s="66">
-        <v>0</v>
-      </c>
-      <c r="N37" s="65">
-        <v>1</v>
-      </c>
-      <c r="R37" t="s">
-        <v>280</v>
-      </c>
-      <c r="S37" t="s">
-        <v>281</v>
-      </c>
-      <c r="T37">
-        <v>10</v>
-      </c>
-      <c r="U37" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="221" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(D38,4) + _xlfn.BITLSHIFT(D$36,12),4)</f>
-        <v>2010</v>
-      </c>
-      <c r="F38" s="266" t="s">
-        <v>344</v>
-      </c>
-      <c r="G38" s="34">
-        <v>4</v>
-      </c>
-      <c r="H38" s="34">
-        <f>ROUNDUP(G38/4,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>175</v>
-      </c>
-      <c r="J38" s="1"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="65"/>
-      <c r="P38" s="274" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F39" s="266"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="65"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F40" s="266"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="66"/>
       <c r="L40" s="66"/>
       <c r="M40" s="66"/>
       <c r="N40" s="65"/>
+      <c r="P40" s="274" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F41" s="266"/>
@@ -14525,146 +15000,74 @@
       <c r="M43" s="66"/>
       <c r="N43" s="65"/>
     </row>
-    <row r="44" spans="1:21" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="217" t="s">
-        <v>279</v>
-      </c>
-      <c r="B44" s="218" t="s">
-        <v>266</v>
-      </c>
-      <c r="C44" s="218" t="s">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F44" s="266"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="65"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F45" s="266"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="66"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="65"/>
+    </row>
+    <row r="46" spans="1:21" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="217" t="s">
         <v>277</v>
       </c>
-      <c r="D44" s="218">
+      <c r="B46" s="218" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="218" t="s">
+        <v>275</v>
+      </c>
+      <c r="D46" s="218">
         <v>3</v>
       </c>
-      <c r="E44" s="220"/>
-      <c r="F44" s="265"/>
-      <c r="G44" s="218">
-        <f>SUM(G45:G59)</f>
+      <c r="E46" s="220"/>
+      <c r="F46" s="265"/>
+      <c r="G46" s="218">
+        <f>SUM(G47:G61)</f>
         <v>30</v>
       </c>
-      <c r="K44" s="263"/>
-      <c r="L44" s="263"/>
-      <c r="M44" s="263"/>
-      <c r="N44" s="263"/>
-      <c r="O44" s="263"/>
-      <c r="P44" s="276"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45" s="221" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(D45,4) + _xlfn.BITLSHIFT(D$44,12),4)</f>
-        <v>3000</v>
-      </c>
-      <c r="F45" s="266" t="s">
-        <v>286</v>
-      </c>
-      <c r="G45" s="34">
-        <v>1</v>
-      </c>
-      <c r="H45" s="34">
-        <f>ROUNDUP(G45/4,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I45" t="s">
-        <v>178</v>
-      </c>
-      <c r="J45" s="1"/>
-      <c r="K45" s="66">
-        <v>0</v>
-      </c>
-      <c r="L45" s="66">
-        <v>1</v>
-      </c>
-      <c r="M45" s="66">
-        <v>0</v>
-      </c>
-      <c r="N45" s="65">
-        <v>1</v>
-      </c>
-      <c r="R45" t="s">
-        <v>280</v>
-      </c>
-      <c r="S45" t="s">
-        <v>311</v>
-      </c>
-      <c r="T45" t="s">
-        <v>312</v>
-      </c>
-      <c r="U45" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="221" t="str">
-        <f t="shared" ref="E46:E59" si="4">DEC2HEX(_xlfn.BITLSHIFT(D46,4) + _xlfn.BITLSHIFT(D$44,12),4)</f>
-        <v>3010</v>
-      </c>
-      <c r="F46" s="266" t="s">
-        <v>287</v>
-      </c>
-      <c r="G46" s="34">
-        <v>1</v>
-      </c>
-      <c r="H46" s="34">
-        <f t="shared" ref="H46:H59" si="5">ROUNDUP(G46/4,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I46" t="s">
-        <v>178</v>
-      </c>
-      <c r="K46" s="66">
-        <v>0</v>
-      </c>
-      <c r="L46" s="66">
-        <v>1</v>
-      </c>
-      <c r="M46" s="66">
-        <v>0</v>
-      </c>
-      <c r="N46" s="65">
-        <v>1</v>
-      </c>
-      <c r="R46" t="s">
-        <v>314</v>
-      </c>
-      <c r="S46" t="s">
-        <v>315</v>
-      </c>
-      <c r="T46" t="s">
-        <v>317</v>
-      </c>
-      <c r="U46" t="s">
-        <v>316</v>
-      </c>
+      <c r="K46" s="263"/>
+      <c r="L46" s="263"/>
+      <c r="M46" s="263"/>
+      <c r="N46" s="263"/>
+      <c r="O46" s="263"/>
+      <c r="P46" s="276"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E47" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3020</v>
+        <f>DEC2HEX(_xlfn.BITLSHIFT(D47,4) + _xlfn.BITLSHIFT(D$46,12),4)</f>
+        <v>3000</v>
       </c>
       <c r="F47" s="266" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="G47" s="34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H47" s="34">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(G47/4,0)</f>
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>175</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="J47" s="1"/>
       <c r="K47" s="66">
         <v>0</v>
       </c>
@@ -14677,20 +15080,26 @@
       <c r="N47" s="65">
         <v>1</v>
       </c>
-      <c r="R47">
-        <v>0</v>
+      <c r="R47" t="s">
+        <v>278</v>
       </c>
       <c r="S47" t="s">
-        <v>281</v>
+        <v>309</v>
+      </c>
+      <c r="T47" t="s">
+        <v>310</v>
+      </c>
+      <c r="U47" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E48" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3030</v>
+        <f t="shared" ref="E48:E61" si="5">DEC2HEX(_xlfn.BITLSHIFT(D48,4) + _xlfn.BITLSHIFT(D$46,12),4)</f>
+        <v>3010</v>
       </c>
       <c r="F48" s="266" t="s">
         <v>285</v>
@@ -14699,7 +15108,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H48:H61" si="6">ROUNDUP(G48/4,0)</f>
         <v>1</v>
       </c>
       <c r="I48" t="s">
@@ -14717,67 +15126,79 @@
       <c r="N48" s="65">
         <v>1</v>
       </c>
-      <c r="R48" s="67" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R48" t="s">
+        <v>312</v>
+      </c>
+      <c r="S48" t="s">
+        <v>313</v>
+      </c>
+      <c r="T48" t="s">
+        <v>315</v>
+      </c>
+      <c r="U48" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" s="221" t="str">
+        <f t="shared" si="5"/>
+        <v>3020</v>
+      </c>
+      <c r="F49" s="266" t="s">
+        <v>294</v>
+      </c>
+      <c r="G49" s="34">
         <v>4</v>
       </c>
-      <c r="E49" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3040</v>
-      </c>
-      <c r="F49" s="266" t="s">
-        <v>289</v>
-      </c>
-      <c r="G49" s="34">
-        <v>1</v>
-      </c>
       <c r="H49" s="34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>175</v>
+      </c>
+      <c r="K49" s="66">
+        <v>0</v>
+      </c>
+      <c r="L49" s="66">
+        <v>1</v>
+      </c>
+      <c r="M49" s="66">
+        <v>0</v>
+      </c>
+      <c r="N49" s="65">
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" s="221" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="I49" t="s">
+        <v>3030</v>
+      </c>
+      <c r="F50" s="266" t="s">
+        <v>283</v>
+      </c>
+      <c r="G50" s="34">
+        <v>1</v>
+      </c>
+      <c r="H50" s="34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
         <v>178</v>
-      </c>
-      <c r="K49" s="66">
-        <v>0</v>
-      </c>
-      <c r="L49" s="66">
-        <v>1</v>
-      </c>
-      <c r="M49" s="66">
-        <v>0</v>
-      </c>
-      <c r="N49" s="65">
-        <v>1</v>
-      </c>
-      <c r="R49" s="67" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D50">
-        <v>5</v>
-      </c>
-      <c r="E50" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3050</v>
-      </c>
-      <c r="F50" s="266" t="s">
-        <v>297</v>
-      </c>
-      <c r="G50" s="34">
-        <v>4</v>
-      </c>
-      <c r="H50" s="34">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="I50" t="s">
-        <v>175</v>
       </c>
       <c r="K50" s="66">
         <v>0</v>
@@ -14795,22 +15216,22 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D51">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E51" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3060</v>
+        <f t="shared" si="5"/>
+        <v>3040</v>
       </c>
       <c r="F51" s="266" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G51" s="34">
         <v>1</v>
       </c>
       <c r="H51" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I51" t="s">
@@ -14832,26 +15253,26 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D52">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E52" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3070</v>
+        <f t="shared" si="5"/>
+        <v>3050</v>
       </c>
       <c r="F52" s="266" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="G52" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H52" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K52" s="66">
         <v>0</v>
@@ -14869,26 +15290,26 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D53">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E53" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3080</v>
+        <f t="shared" si="5"/>
+        <v>3060</v>
       </c>
       <c r="F53" s="266" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="G53" s="34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H53" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="K53" s="66">
         <v>0</v>
@@ -14906,22 +15327,22 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D54">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E54" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>3090</v>
+        <f t="shared" si="5"/>
+        <v>3070</v>
       </c>
       <c r="F54" s="266" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G54" s="34">
         <v>1</v>
       </c>
       <c r="H54" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I54" t="s">
@@ -14943,26 +15364,26 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D55">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E55" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>30A0</v>
+        <f t="shared" si="5"/>
+        <v>3080</v>
       </c>
       <c r="F55" s="266" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="G55" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H55" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K55" s="66">
         <v>0</v>
@@ -14980,26 +15401,26 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D56">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E56" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>30B0</v>
+        <f t="shared" si="5"/>
+        <v>3090</v>
       </c>
       <c r="F56" s="266" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="G56" s="34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H56" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="K56" s="66">
         <v>0</v>
@@ -15017,22 +15438,22 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D57">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E57" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>30C0</v>
+        <f t="shared" si="5"/>
+        <v>30A0</v>
       </c>
       <c r="F57" s="266" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G57" s="34">
         <v>1</v>
       </c>
       <c r="H57" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I57" t="s">
@@ -15054,26 +15475,26 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D58">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E58" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>30D0</v>
+        <f t="shared" si="5"/>
+        <v>30B0</v>
       </c>
       <c r="F58" s="266" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G58" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H58" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K58" s="66">
         <v>0</v>
@@ -15091,26 +15512,26 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D59">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E59" s="221" t="str">
-        <f t="shared" si="4"/>
-        <v>30E0</v>
+        <f t="shared" si="5"/>
+        <v>30C0</v>
       </c>
       <c r="F59" s="266" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="G59" s="34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H59" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="K59" s="66">
         <v>0</v>
@@ -15128,104 +15549,172 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F60" s="266"/>
-    </row>
-    <row r="61" spans="1:18" s="218" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="218" t="s">
-        <v>279</v>
-      </c>
-      <c r="B61" s="218" t="s">
-        <v>266</v>
-      </c>
-      <c r="C61" s="218" t="s">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>13</v>
+      </c>
+      <c r="E60" s="221" t="str">
+        <f t="shared" si="5"/>
+        <v>30D0</v>
+      </c>
+      <c r="F60" s="266" t="s">
+        <v>292</v>
+      </c>
+      <c r="G60" s="34">
+        <v>1</v>
+      </c>
+      <c r="H60" s="34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>178</v>
+      </c>
+      <c r="K60" s="66">
+        <v>0</v>
+      </c>
+      <c r="L60" s="66">
+        <v>1</v>
+      </c>
+      <c r="M60" s="66">
+        <v>0</v>
+      </c>
+      <c r="N60" s="65">
+        <v>1</v>
+      </c>
+      <c r="R60" s="67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>14</v>
+      </c>
+      <c r="E61" s="221" t="str">
+        <f t="shared" si="5"/>
+        <v>30E0</v>
+      </c>
+      <c r="F61" s="266" t="s">
+        <v>298</v>
+      </c>
+      <c r="G61" s="34">
+        <v>4</v>
+      </c>
+      <c r="H61" s="34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>175</v>
+      </c>
+      <c r="K61" s="66">
+        <v>0</v>
+      </c>
+      <c r="L61" s="66">
+        <v>1</v>
+      </c>
+      <c r="M61" s="66">
+        <v>0</v>
+      </c>
+      <c r="N61" s="65">
+        <v>1</v>
+      </c>
+      <c r="R61" s="67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F62" s="266"/>
+    </row>
+    <row r="63" spans="1:19" s="218" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="218" t="s">
         <v>277</v>
       </c>
-      <c r="D61" s="218">
+      <c r="B63" s="218" t="s">
+        <v>264</v>
+      </c>
+      <c r="C63" s="218" t="s">
+        <v>275</v>
+      </c>
+      <c r="D63" s="218">
         <v>4</v>
       </c>
-      <c r="E61" s="220"/>
-      <c r="F61" s="265"/>
-      <c r="G61" s="218">
-        <f>SUM(G62:G63)</f>
-        <v>0</v>
-      </c>
-      <c r="K61" s="263"/>
-      <c r="L61" s="263"/>
-      <c r="M61" s="263"/>
-      <c r="N61" s="263"/>
-      <c r="O61" s="263"/>
-      <c r="P61" s="276"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62" s="221" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(D62,4) + _xlfn.BITLSHIFT(D$61,12),4)</f>
+      <c r="E63" s="220"/>
+      <c r="F63" s="265"/>
+      <c r="G63" s="218">
+        <f>SUM(G64:G65)</f>
+        <v>0</v>
+      </c>
+      <c r="K63" s="263"/>
+      <c r="L63" s="263"/>
+      <c r="M63" s="263"/>
+      <c r="N63" s="263"/>
+      <c r="O63" s="263"/>
+      <c r="P63" s="276"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" s="221" t="str">
+        <f>DEC2HEX(_xlfn.BITLSHIFT(D64,4) + _xlfn.BITLSHIFT(D$63,12),4)</f>
         <v>4000</v>
       </c>
-      <c r="F62" s="266"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63" s="221" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(D63,4) + _xlfn.BITLSHIFT(D$61,12),4)</f>
+      <c r="F64" s="266"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" s="221" t="str">
+        <f>DEC2HEX(_xlfn.BITLSHIFT(D65,4) + _xlfn.BITLSHIFT(D$63,12),4)</f>
         <v>4010</v>
       </c>
-      <c r="F63" s="266"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F64" s="266"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65" s="266"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F66" s="266"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F67" s="266"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F68" s="266"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F69" s="266"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F70" s="266"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F71" s="266"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F72" s="266"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F73" s="266"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F74" s="266"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F75" s="266"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F76" s="266"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F77" s="266"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F78" s="266"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F79" s="266"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F80" s="266"/>
     </row>
     <row r="81" spans="6:6" x14ac:dyDescent="0.25">
@@ -16130,6 +16619,12 @@
     </row>
     <row r="381" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F381" s="266"/>
+    </row>
+    <row r="382" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F382" s="266"/>
+    </row>
+    <row r="383" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F383" s="266"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactored caniot, updated arch
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECBD3BE-C8AE-4BAE-A4E2-E4384B3FB08A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B183EF-72C7-4FA4-997E-802B0ABDF21D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
   <sheets>
     <sheet name="frames-data-bits" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="355">
   <si>
     <t>temperature</t>
   </si>
@@ -1068,12 +1068,6 @@
     <t>sent.telemetry</t>
   </si>
   <si>
-    <t>telemetry request random period</t>
-  </si>
-  <si>
-    <t>random period between 0 and value when requesting telemetry in broadcast</t>
-  </si>
-  <si>
     <t>calculated_abstime</t>
   </si>
   <si>
@@ -1096,6 +1090,21 @@
   </si>
   <si>
     <t>TempSensDev</t>
+  </si>
+  <si>
+    <t>telemetry_min</t>
+  </si>
+  <si>
+    <t>random period between 0 and value when requesting telemetry when broadcast</t>
+  </si>
+  <si>
+    <t>telemetry_rdm_delay</t>
+  </si>
+  <si>
+    <t>lfsr32</t>
+  </si>
+  <si>
+    <t>lfsr31</t>
   </si>
 </sst>
 </file>
@@ -9523,8 +9532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36880ADF-04C9-4A12-8EFC-224812D037A0}">
   <dimension ref="A3:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P58" sqref="P58"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9993,7 +10002,7 @@
         <v>2</v>
       </c>
       <c r="M23" s="279" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -10682,7 +10691,7 @@
         <v>258</v>
       </c>
       <c r="K48" s="259" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L48" s="277">
         <v>3</v>
@@ -10710,7 +10719,7 @@
         <v>258</v>
       </c>
       <c r="K49" s="259" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L49" s="277">
         <v>3</v>
@@ -10738,7 +10747,7 @@
         <v>258</v>
       </c>
       <c r="K50" s="259" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L50" s="277">
         <v>3</v>
@@ -11104,7 +11113,7 @@
         <v>260</v>
       </c>
       <c r="K64" s="258" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L64" s="277">
         <v>5</v>
@@ -13763,8 +13772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
   <dimension ref="A1:V383"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13773,7 +13782,7 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="221" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="222" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="222" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
@@ -14232,7 +14241,7 @@
         <v>1020</v>
       </c>
       <c r="F18" s="266" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G18" s="34">
         <v>4</v>
@@ -14667,7 +14676,7 @@
         <v>10E0</v>
       </c>
       <c r="F30" s="266" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G30" s="34">
         <v>4</v>
@@ -14772,7 +14781,7 @@
         <v>1110</v>
       </c>
       <c r="F33" s="266" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G33" s="34">
         <v>2</v>
@@ -14884,7 +14893,7 @@
       <c r="F38" s="265"/>
       <c r="G38" s="218">
         <f>SUM(G39:G44)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K38" s="263"/>
       <c r="L38" s="263"/>
@@ -14949,7 +14958,7 @@
         <v>2010</v>
       </c>
       <c r="F40" s="266" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="G40" s="34">
         <v>4</v>
@@ -14962,43 +14971,135 @@
         <v>175</v>
       </c>
       <c r="J40" s="1"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="65"/>
+      <c r="K40" s="66">
+        <v>0</v>
+      </c>
+      <c r="L40" s="66">
+        <v>1</v>
+      </c>
+      <c r="M40" s="66">
+        <v>0</v>
+      </c>
+      <c r="N40" s="65">
+        <v>1</v>
+      </c>
       <c r="P40" s="274" t="s">
-        <v>343</v>
+        <v>351</v>
+      </c>
+      <c r="R40" t="s">
+        <v>278</v>
+      </c>
+      <c r="S40" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F41" s="266"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" s="221" t="str">
+        <f>DEC2HEX(_xlfn.BITLSHIFT(D41,4) + _xlfn.BITLSHIFT(D$38,12),4)</f>
+        <v>2020</v>
+      </c>
+      <c r="F41" s="266" t="s">
+        <v>350</v>
+      </c>
+      <c r="G41" s="34">
+        <v>4</v>
+      </c>
+      <c r="H41" s="34">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>175</v>
+      </c>
       <c r="J41" s="1"/>
-      <c r="K41" s="66"/>
-      <c r="L41" s="66"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="65"/>
+      <c r="K41" s="66">
+        <v>0</v>
+      </c>
+      <c r="L41" s="66">
+        <v>1</v>
+      </c>
+      <c r="M41" s="66">
+        <v>0</v>
+      </c>
+      <c r="N41" s="65">
+        <v>1</v>
+      </c>
+      <c r="R41" t="s">
+        <v>278</v>
+      </c>
+      <c r="S41" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F42" s="266"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42" s="221" t="str">
+        <f t="shared" ref="E42:E43" si="5">DEC2HEX(_xlfn.BITLSHIFT(D42,4) + _xlfn.BITLSHIFT(D$38,12),4)</f>
+        <v>2030</v>
+      </c>
+      <c r="F42" s="266" t="s">
+        <v>353</v>
+      </c>
+      <c r="G42" s="34">
+        <v>4</v>
+      </c>
+      <c r="H42" s="34">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>175</v>
+      </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="65"/>
+      <c r="K42" s="66">
+        <v>0</v>
+      </c>
+      <c r="L42" s="66">
+        <v>1</v>
+      </c>
+      <c r="M42" s="66">
+        <v>0</v>
+      </c>
+      <c r="N42" s="65">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F43" s="266"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43" s="221" t="str">
+        <f t="shared" si="5"/>
+        <v>2040</v>
+      </c>
+      <c r="F43" s="266" t="s">
+        <v>354</v>
+      </c>
+      <c r="G43" s="34">
+        <v>4</v>
+      </c>
+      <c r="H43" s="34">
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>175</v>
+      </c>
       <c r="J43" s="1"/>
-      <c r="K43" s="66"/>
-      <c r="L43" s="66"/>
-      <c r="M43" s="66"/>
-      <c r="N43" s="65"/>
+      <c r="K43" s="66">
+        <v>0</v>
+      </c>
+      <c r="L43" s="66">
+        <v>1</v>
+      </c>
+      <c r="M43" s="66">
+        <v>0</v>
+      </c>
+      <c r="N43" s="65">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F44" s="266"/>
@@ -15098,7 +15199,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="221" t="str">
-        <f t="shared" ref="E48:E61" si="5">DEC2HEX(_xlfn.BITLSHIFT(D48,4) + _xlfn.BITLSHIFT(D$46,12),4)</f>
+        <f t="shared" ref="E48:E61" si="6">DEC2HEX(_xlfn.BITLSHIFT(D48,4) + _xlfn.BITLSHIFT(D$46,12),4)</f>
         <v>3010</v>
       </c>
       <c r="F48" s="266" t="s">
@@ -15108,7 +15209,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="34">
-        <f t="shared" ref="H48:H61" si="6">ROUNDUP(G48/4,0)</f>
+        <f t="shared" ref="H48:H61" si="7">ROUNDUP(G48/4,0)</f>
         <v>1</v>
       </c>
       <c r="I48" t="s">
@@ -15144,7 +15245,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3020</v>
       </c>
       <c r="F49" s="266" t="s">
@@ -15154,7 +15255,7 @@
         <v>4</v>
       </c>
       <c r="H49" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I49" t="s">
@@ -15184,7 +15285,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3030</v>
       </c>
       <c r="F50" s="266" t="s">
@@ -15194,7 +15295,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I50" t="s">
@@ -15221,7 +15322,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3040</v>
       </c>
       <c r="F51" s="266" t="s">
@@ -15231,7 +15332,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I51" t="s">
@@ -15258,7 +15359,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3050</v>
       </c>
       <c r="F52" s="266" t="s">
@@ -15268,7 +15369,7 @@
         <v>4</v>
       </c>
       <c r="H52" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I52" t="s">
@@ -15295,7 +15396,7 @@
         <v>6</v>
       </c>
       <c r="E53" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3060</v>
       </c>
       <c r="F53" s="266" t="s">
@@ -15305,7 +15406,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I53" t="s">
@@ -15332,7 +15433,7 @@
         <v>7</v>
       </c>
       <c r="E54" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3070</v>
       </c>
       <c r="F54" s="266" t="s">
@@ -15342,7 +15443,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I54" t="s">
@@ -15369,7 +15470,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3080</v>
       </c>
       <c r="F55" s="266" t="s">
@@ -15379,7 +15480,7 @@
         <v>4</v>
       </c>
       <c r="H55" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I55" t="s">
@@ -15406,7 +15507,7 @@
         <v>9</v>
       </c>
       <c r="E56" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3090</v>
       </c>
       <c r="F56" s="266" t="s">
@@ -15416,7 +15517,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I56" t="s">
@@ -15443,7 +15544,7 @@
         <v>10</v>
       </c>
       <c r="E57" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30A0</v>
       </c>
       <c r="F57" s="266" t="s">
@@ -15453,7 +15554,7 @@
         <v>1</v>
       </c>
       <c r="H57" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I57" t="s">
@@ -15480,7 +15581,7 @@
         <v>11</v>
       </c>
       <c r="E58" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30B0</v>
       </c>
       <c r="F58" s="266" t="s">
@@ -15490,7 +15591,7 @@
         <v>4</v>
       </c>
       <c r="H58" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I58" t="s">
@@ -15517,7 +15618,7 @@
         <v>12</v>
       </c>
       <c r="E59" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30C0</v>
       </c>
       <c r="F59" s="266" t="s">
@@ -15527,7 +15628,7 @@
         <v>1</v>
       </c>
       <c r="H59" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I59" t="s">
@@ -15554,7 +15655,7 @@
         <v>13</v>
       </c>
       <c r="E60" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30D0</v>
       </c>
       <c r="F60" s="266" t="s">
@@ -15564,7 +15665,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I60" t="s">
@@ -15591,7 +15692,7 @@
         <v>14</v>
       </c>
       <c r="E61" s="221" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30E0</v>
       </c>
       <c r="F61" s="266" t="s">
@@ -15601,7 +15702,7 @@
         <v>4</v>
       </c>
       <c r="H61" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I61" t="s">

</xml_diff>

<commit_message>
Set CANIOT version 1.10
</commit_message>
<xml_diff>
--- a/docs/arch.xlsx
+++ b/docs/arch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ProjetsRecherche\Embedded\CAN\dev\caniot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B183EF-72C7-4FA4-997E-802B0ABDF21D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A31D46-CAAB-4FB9-89B0-50ACCEE27F72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F2F15D1-277A-4EC5-A845-66E8BFF58C30}"/>
   </bookViews>
   <sheets>
     <sheet name="frames-data-bits" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="362">
   <si>
     <t>temperature</t>
   </si>
@@ -783,9 +783,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>Data type</t>
   </si>
   <si>
@@ -1011,9 +1008,6 @@
     <t>special</t>
   </si>
   <si>
-    <t>255 (section</t>
-  </si>
-  <si>
     <t>size (B)</t>
   </si>
   <si>
@@ -1105,6 +1099,33 @@
   </si>
   <si>
     <t>lfsr31</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>3*1000</t>
+  </si>
+  <si>
+    <t>1*1000</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>FakeDevice</t>
+  </si>
+  <si>
+    <t>00.00</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To </t>
+  </si>
+  <si>
+    <t>Invalid</t>
   </si>
 </sst>
 </file>
@@ -1635,7 +1656,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="282">
+  <cellXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2338,6 +2359,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2837,8 +2859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABEE202-717B-4A96-9406-D9A14283F0F2}">
   <dimension ref="B1:AH59"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="W53" sqref="W53"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3183,28 +3205,28 @@
         <v>81</v>
       </c>
       <c r="N13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="S13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="U13" s="167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="V13" s="25" t="s">
         <v>45</v>
@@ -3996,7 +4018,7 @@
         <v>153</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -4562,7 +4584,7 @@
         <v>152</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
@@ -4575,7 +4597,7 @@
       <c r="L40" s="48"/>
       <c r="M40" s="48"/>
       <c r="T40" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="2:34" x14ac:dyDescent="0.2">
@@ -4605,7 +4627,7 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>144</v>
@@ -5128,7 +5150,7 @@
     </row>
     <row r="52" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>15</v>
@@ -5253,76 +5275,76 @@
     </row>
     <row r="55" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C55" s="268" t="s">
+        <v>316</v>
+      </c>
+      <c r="D55" s="268" t="s">
+        <v>316</v>
+      </c>
+      <c r="E55" s="268" t="s">
+        <v>316</v>
+      </c>
+      <c r="F55" s="268" t="s">
+        <v>316</v>
+      </c>
+      <c r="G55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="H55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="I55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="J55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="K55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="L55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="M55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="N55" s="269" t="s">
+        <v>251</v>
+      </c>
+      <c r="O55" s="270" t="s">
         <v>317</v>
       </c>
-      <c r="D55" s="268" t="s">
+      <c r="P55" s="270" t="s">
         <v>317</v>
       </c>
-      <c r="E55" s="268" t="s">
+      <c r="Q55" s="270" t="s">
         <v>317</v>
       </c>
-      <c r="F55" s="268" t="s">
+      <c r="R55" s="270" t="s">
         <v>317</v>
-      </c>
-      <c r="G55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="H55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="I55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="J55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="K55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="L55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="M55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="N55" s="269" t="s">
-        <v>252</v>
-      </c>
-      <c r="O55" s="270" t="s">
-        <v>318</v>
-      </c>
-      <c r="P55" s="270" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q55" s="270" t="s">
-        <v>318</v>
-      </c>
-      <c r="R55" s="270" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="57" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C57" s="268" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C58" s="269" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C59" s="270" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5352,7 +5374,7 @@
   <sheetData>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>156</v>
@@ -5443,7 +5465,7 @@
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A3" s="247" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>83</v>
@@ -5648,207 +5670,207 @@
     <row r="4" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A4" s="245"/>
       <c r="B4" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C4" s="239">
         <v>8</v>
       </c>
       <c r="D4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="W4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="X4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Y4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AA4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AB4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AC4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AD4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AE4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AF4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AG4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AH4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AI4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AJ4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AK4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AL4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AM4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AN4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AO4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AP4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AQ4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AR4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AS4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AT4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AU4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AV4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AW4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AX4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AY4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AZ4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BA4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BB4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BC4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BD4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BE4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BF4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BG4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BH4" s="241" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BI4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BJ4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BK4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BL4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BM4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BN4" s="242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BO4" s="243" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A6" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>156</v>
@@ -5939,7 +5961,7 @@
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A7" s="246" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>82</v>
@@ -6144,7 +6166,7 @@
     <row r="8" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A8" s="245"/>
       <c r="B8" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C8" s="239">
         <v>1</v>
@@ -6344,7 +6366,7 @@
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A10" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>156</v>
@@ -6435,7 +6457,7 @@
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A11" s="247" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>82</v>
@@ -6640,7 +6662,7 @@
     <row r="12" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A12" s="245"/>
       <c r="B12" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" s="239">
         <v>4</v>
@@ -6712,34 +6734,34 @@
         <v>46</v>
       </c>
       <c r="Z12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AA12" s="238" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AB12" s="187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AC12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AD12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AE12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AF12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AG12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AH12" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AI12" s="238" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AJ12" s="184" t="s">
         <v>46</v>
@@ -6874,7 +6896,7 @@
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A14" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>156</v>
@@ -6965,7 +6987,7 @@
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A15" s="247" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>83</v>
@@ -7170,7 +7192,7 @@
     <row r="16" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A16" s="245"/>
       <c r="B16" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C16" s="239">
         <v>4</v>
@@ -7404,7 +7426,7 @@
     </row>
     <row r="18" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A18" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -7495,7 +7517,7 @@
     </row>
     <row r="19" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A19" s="247" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>83</v>
@@ -7700,7 +7722,7 @@
     <row r="20" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A20" s="245"/>
       <c r="B20" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C20" s="239">
         <v>8</v>
@@ -7850,34 +7872,34 @@
         <v>25</v>
       </c>
       <c r="AZ20" s="187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BA20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BB20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BC20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BD20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BE20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BF20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BG20" s="238" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BH20" s="187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BI20" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BJ20" s="185" t="s">
         <v>46</v>
@@ -7934,7 +7956,7 @@
     </row>
     <row r="22" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A22" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>156</v>
@@ -8025,7 +8047,7 @@
     </row>
     <row r="23" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A23" s="247" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>83</v>
@@ -8230,7 +8252,7 @@
     <row r="24" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A24" s="245"/>
       <c r="B24" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C24" s="239">
         <v>8</v>
@@ -8332,94 +8354,94 @@
         <v>24</v>
       </c>
       <c r="AJ24" s="187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AK24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AL24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AM24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AN24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AO24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AP24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AQ24" s="238" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AR24" s="187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AS24" s="188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AT24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="AV24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="AX24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="AY24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="AZ24" s="187" t="s">
+        <v>253</v>
+      </c>
+      <c r="BA24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="BB24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="BC24" s="188" t="s">
+        <v>253</v>
+      </c>
+      <c r="BD24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="AU24" s="188" t="s">
+      <c r="BE24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="AV24" s="188" t="s">
+      <c r="BF24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="AW24" s="188" t="s">
+      <c r="BG24" s="238" t="s">
         <v>254</v>
       </c>
-      <c r="AX24" s="188" t="s">
+      <c r="BH24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="AY24" s="188" t="s">
+      <c r="BI24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="AZ24" s="187" t="s">
+      <c r="BJ24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="BA24" s="188" t="s">
+      <c r="BK24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="BB24" s="188" t="s">
+      <c r="BL24" s="188" t="s">
         <v>254</v>
       </c>
-      <c r="BC24" s="188" t="s">
+      <c r="BM24" s="188" t="s">
         <v>254</v>
-      </c>
-      <c r="BD24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BE24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BF24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BG24" s="238" t="s">
-        <v>255</v>
-      </c>
-      <c r="BH24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BI24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BJ24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BK24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BL24" s="188" t="s">
-        <v>255</v>
-      </c>
-      <c r="BM24" s="188" t="s">
-        <v>255</v>
       </c>
       <c r="BN24" s="185" t="s">
         <v>46</v>
@@ -8430,7 +8452,7 @@
     </row>
     <row r="26" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A26" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>156</v>
@@ -8521,7 +8543,7 @@
     </row>
     <row r="27" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A27" s="247" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>83</v>
@@ -8726,7 +8748,7 @@
     <row r="28" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A28" s="245"/>
       <c r="B28" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C28" s="239">
         <v>8</v>
@@ -8876,52 +8898,52 @@
         <v>26</v>
       </c>
       <c r="AZ28" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BA28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BB28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BC28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BD28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BE28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BF28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BG28" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BH28" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BI28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BJ28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BK28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BL28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BM28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BN28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BO28" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:67" x14ac:dyDescent="0.2">
@@ -8960,7 +8982,7 @@
     </row>
     <row r="30" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A30" s="244" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>156</v>
@@ -9256,7 +9278,7 @@
     <row r="32" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A32" s="245"/>
       <c r="B32" s="235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C32" s="239">
         <v>0</v>
@@ -9533,7 +9555,7 @@
   <dimension ref="A3:M93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9605,7 +9627,7 @@
         <v>8</v>
       </c>
       <c r="K4" s="256" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9769,7 +9791,7 @@
         <v>45</v>
       </c>
       <c r="K11" s="256" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -9993,16 +10015,16 @@
         <v>57</v>
       </c>
       <c r="I23" s="64" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K23" s="257" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L23" s="278" t="s">
         <v>2</v>
       </c>
       <c r="M23" s="279" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -10067,7 +10089,7 @@
         <v>84</v>
       </c>
       <c r="I25" s="248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K25" s="258"/>
       <c r="L25" s="35">
@@ -10101,7 +10123,7 @@
       </c>
       <c r="H26" s="86"/>
       <c r="I26" s="248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K26" s="258"/>
       <c r="L26" s="35">
@@ -10130,7 +10152,7 @@
       </c>
       <c r="H27" s="86"/>
       <c r="I27" s="248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K27" s="258"/>
       <c r="L27" s="35">
@@ -10157,7 +10179,7 @@
       </c>
       <c r="H28" s="88"/>
       <c r="I28" s="248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K28" s="259"/>
       <c r="L28" s="35">
@@ -10184,7 +10206,7 @@
       </c>
       <c r="H29" s="88"/>
       <c r="I29" s="248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K29" s="259"/>
       <c r="L29" s="35">
@@ -10211,7 +10233,7 @@
       </c>
       <c r="H30" s="88"/>
       <c r="I30" s="248" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K30" s="259"/>
       <c r="L30" s="35">
@@ -10238,9 +10260,11 @@
       </c>
       <c r="H31" s="88"/>
       <c r="I31" s="248" t="s">
-        <v>256</v>
-      </c>
-      <c r="K31" s="259"/>
+        <v>255</v>
+      </c>
+      <c r="K31" s="259" t="s">
+        <v>357</v>
+      </c>
       <c r="L31" s="35">
         <v>0</v>
       </c>
@@ -10265,7 +10289,7 @@
       </c>
       <c r="H32" s="88"/>
       <c r="I32" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K32" s="259"/>
       <c r="L32" s="277">
@@ -10292,7 +10316,7 @@
       </c>
       <c r="H33" s="88"/>
       <c r="I33" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K33" s="259"/>
       <c r="L33" s="277">
@@ -10319,7 +10343,7 @@
       </c>
       <c r="H34" s="88"/>
       <c r="I34" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K34" s="259"/>
       <c r="L34" s="277">
@@ -10346,7 +10370,7 @@
       </c>
       <c r="H35" s="88"/>
       <c r="I35" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K35" s="259"/>
       <c r="L35" s="277">
@@ -10373,7 +10397,7 @@
       </c>
       <c r="H36" s="88"/>
       <c r="I36" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K36" s="259"/>
       <c r="L36" s="277">
@@ -10400,7 +10424,7 @@
       </c>
       <c r="H37" s="88"/>
       <c r="I37" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K37" s="259"/>
       <c r="L37" s="277">
@@ -10427,7 +10451,7 @@
       </c>
       <c r="H38" s="85"/>
       <c r="I38" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K38" s="259"/>
       <c r="L38" s="277">
@@ -10454,7 +10478,7 @@
       </c>
       <c r="H39" s="89"/>
       <c r="I39" s="249" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K39" s="259"/>
       <c r="L39" s="277">
@@ -10480,7 +10504,7 @@
         <v>179</v>
       </c>
       <c r="I40" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K40" s="259"/>
       <c r="L40" s="277">
@@ -10506,7 +10530,7 @@
         <v>180</v>
       </c>
       <c r="I41" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K41" s="259"/>
       <c r="L41" s="277">
@@ -10532,7 +10556,7 @@
         <v>181</v>
       </c>
       <c r="I42" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K42" s="259"/>
       <c r="L42" s="277">
@@ -10558,7 +10582,7 @@
         <v>182</v>
       </c>
       <c r="I43" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K43" s="259"/>
       <c r="L43" s="277">
@@ -10584,7 +10608,7 @@
         <v>183</v>
       </c>
       <c r="I44" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K44" s="259"/>
       <c r="L44" s="277">
@@ -10610,7 +10634,7 @@
         <v>184</v>
       </c>
       <c r="I45" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K45" s="259"/>
       <c r="L45" s="277">
@@ -10636,7 +10660,7 @@
         <v>185</v>
       </c>
       <c r="I46" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K46" s="259"/>
       <c r="L46" s="277">
@@ -10662,7 +10686,7 @@
         <v>186</v>
       </c>
       <c r="I47" s="250" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K47" s="259"/>
       <c r="L47" s="277">
@@ -10688,10 +10712,10 @@
         <v>187</v>
       </c>
       <c r="I48" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K48" s="259" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L48" s="277">
         <v>3</v>
@@ -10716,10 +10740,10 @@
         <v>188</v>
       </c>
       <c r="I49" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K49" s="259" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L49" s="277">
         <v>3</v>
@@ -10744,10 +10768,10 @@
         <v>189</v>
       </c>
       <c r="I50" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K50" s="259" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L50" s="277">
         <v>3</v>
@@ -10772,7 +10796,7 @@
         <v>190</v>
       </c>
       <c r="I51" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K51" s="259"/>
       <c r="L51" s="277">
@@ -10798,7 +10822,7 @@
         <v>191</v>
       </c>
       <c r="I52" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K52" s="259"/>
       <c r="L52" s="277">
@@ -10824,7 +10848,7 @@
         <v>192</v>
       </c>
       <c r="I53" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K53" s="259"/>
       <c r="L53" s="277">
@@ -10850,7 +10874,7 @@
         <v>193</v>
       </c>
       <c r="I54" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K54" s="259"/>
       <c r="L54" s="277">
@@ -10876,7 +10900,7 @@
         <v>194</v>
       </c>
       <c r="I55" s="249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K55" s="259"/>
       <c r="L55" s="277">
@@ -10902,7 +10926,7 @@
         <v>195</v>
       </c>
       <c r="I56" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K56" s="259"/>
       <c r="L56" s="277">
@@ -10928,7 +10952,7 @@
         <v>196</v>
       </c>
       <c r="I57" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K57" s="259"/>
       <c r="L57" s="277">
@@ -10954,7 +10978,7 @@
         <v>197</v>
       </c>
       <c r="I58" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K58" s="259"/>
       <c r="L58" s="277">
@@ -10980,7 +11004,7 @@
         <v>198</v>
       </c>
       <c r="I59" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K59" s="259"/>
       <c r="L59" s="277">
@@ -11006,7 +11030,7 @@
         <v>199</v>
       </c>
       <c r="I60" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K60" s="259"/>
       <c r="L60" s="277">
@@ -11032,7 +11056,7 @@
         <v>200</v>
       </c>
       <c r="I61" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K61" s="259"/>
       <c r="L61" s="277">
@@ -11058,7 +11082,7 @@
         <v>201</v>
       </c>
       <c r="I62" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K62" s="259"/>
       <c r="L62" s="277">
@@ -11084,7 +11108,7 @@
         <v>202</v>
       </c>
       <c r="I63" s="249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K63" s="259"/>
       <c r="L63" s="277">
@@ -11110,10 +11134,10 @@
         <v>203</v>
       </c>
       <c r="I64" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K64" s="258" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L64" s="277">
         <v>5</v>
@@ -11138,7 +11162,7 @@
         <v>204</v>
       </c>
       <c r="I65" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K65" s="259"/>
       <c r="L65" s="277">
@@ -11164,7 +11188,7 @@
         <v>205</v>
       </c>
       <c r="I66" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K66" s="259"/>
       <c r="L66" s="277">
@@ -11190,7 +11214,7 @@
         <v>206</v>
       </c>
       <c r="I67" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K67" s="259"/>
       <c r="L67" s="277">
@@ -11216,7 +11240,7 @@
         <v>207</v>
       </c>
       <c r="I68" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K68" s="259"/>
       <c r="L68" s="277">
@@ -11242,7 +11266,7 @@
         <v>208</v>
       </c>
       <c r="I69" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K69" s="259"/>
       <c r="L69" s="277">
@@ -11268,7 +11292,7 @@
         <v>209</v>
       </c>
       <c r="I70" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K70" s="259"/>
       <c r="L70" s="277">
@@ -11294,7 +11318,7 @@
         <v>210</v>
       </c>
       <c r="I71" s="249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K71" s="259"/>
       <c r="L71" s="277">
@@ -11320,7 +11344,7 @@
         <v>211</v>
       </c>
       <c r="I72" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K72" s="259"/>
       <c r="L72" s="277">
@@ -11346,7 +11370,7 @@
         <v>212</v>
       </c>
       <c r="I73" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K73" s="259"/>
       <c r="L73" s="277">
@@ -11372,7 +11396,7 @@
         <v>213</v>
       </c>
       <c r="I74" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K74" s="259"/>
       <c r="L74" s="277">
@@ -11398,7 +11422,7 @@
         <v>214</v>
       </c>
       <c r="I75" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K75" s="259"/>
       <c r="L75" s="277">
@@ -11424,7 +11448,7 @@
         <v>215</v>
       </c>
       <c r="I76" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K76" s="259"/>
       <c r="L76" s="277">
@@ -11450,7 +11474,7 @@
         <v>216</v>
       </c>
       <c r="I77" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K77" s="259"/>
       <c r="L77" s="277">
@@ -11476,7 +11500,7 @@
         <v>217</v>
       </c>
       <c r="I78" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K78" s="259"/>
       <c r="L78" s="277">
@@ -11502,7 +11526,7 @@
         <v>218</v>
       </c>
       <c r="I79" s="249" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K79" s="259"/>
       <c r="L79" s="277">
@@ -11729,7 +11753,7 @@
         <v>55</v>
       </c>
       <c r="B89" s="59" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C89" s="60"/>
       <c r="D89" s="63" t="s">
@@ -11757,7 +11781,7 @@
         <v>54</v>
       </c>
       <c r="B90" s="271" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C90" s="52"/>
       <c r="D90" s="272">
@@ -11827,13 +11851,13 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D93" s="67" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E93" s="67" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F93" s="67" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -12127,28 +12151,28 @@
         <v>81</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="R8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="S8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="U8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="V8" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="W8" s="25" t="s">
         <v>45</v>
@@ -12776,10 +12800,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="237" t="s">
         <v>251</v>
-      </c>
-      <c r="C7" s="237" t="s">
-        <v>252</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -12944,7 +12968,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13052,7 +13076,7 @@
       <c r="S4" s="94"/>
       <c r="T4" s="95"/>
       <c r="V4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -13107,12 +13131,12 @@
         <v>126</v>
       </c>
       <c r="V5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="V6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -13575,13 +13599,13 @@
         <v>123</v>
       </c>
       <c r="Q14" s="49" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="R14" s="49" t="s">
         <v>124</v>
       </c>
       <c r="S14" s="49" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="T14" s="97" t="s">
         <v>148</v>
@@ -13651,7 +13675,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="212" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C16" s="96">
         <v>0</v>
@@ -13690,7 +13714,7 @@
         <v>104</v>
       </c>
       <c r="P16" s="262" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q16" s="262" t="s">
         <v>115</v>
@@ -13705,27 +13729,27 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="C17" s="96">
-        <v>1</v>
-      </c>
-      <c r="D17" s="97">
-        <v>0</v>
+      <c r="C17" s="96" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" s="97" t="s">
+        <v>359</v>
       </c>
       <c r="E17" s="58">
-        <v>0</v>
-      </c>
-      <c r="F17" s="96">
-        <v>1</v>
-      </c>
-      <c r="G17" s="97">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F17" s="96" t="s">
+        <v>359</v>
+      </c>
+      <c r="G17" s="97" t="s">
+        <v>359</v>
       </c>
       <c r="H17" s="96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="262">
         <v>1</v>
@@ -13734,37 +13758,59 @@
         <v>1</v>
       </c>
       <c r="K17" s="262">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="262">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O17" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="P17" s="262" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q17" s="262" t="s">
+        <v>360</v>
+      </c>
+      <c r="R17" s="262" t="s">
+        <v>106</v>
+      </c>
+      <c r="S17" s="262" t="s">
+        <v>120</v>
+      </c>
+      <c r="T17" s="97" t="s">
+        <v>148</v>
+      </c>
+      <c r="U17" s="282" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13772,8 +13818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440C4F6B-A1C2-4D6C-BCC9-98B3358D661D}">
   <dimension ref="A1:V383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13794,6 +13840,7 @@
     <col min="17" max="17" width="7" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -13810,7 +13857,7 @@
         <v>157</v>
       </c>
       <c r="G1" s="63" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>161</v>
@@ -13840,7 +13887,7 @@
         <v>173</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="218" customFormat="1" x14ac:dyDescent="0.25">
@@ -13848,7 +13895,7 @@
         <v>160</v>
       </c>
       <c r="C2" s="218" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D2" s="218">
         <v>0</v>
@@ -13860,13 +13907,13 @@
         <v>35</v>
       </c>
       <c r="K2" s="263" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L2" s="263" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M2" s="263" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N2" s="263" t="s">
         <v>88</v>
@@ -13963,7 +14010,7 @@
         <v>100</v>
       </c>
       <c r="U4" t="s">
-        <v>247</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -13975,7 +14022,7 @@
         <v>0020</v>
       </c>
       <c r="F5" s="266" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G5" s="34">
         <v>32</v>
@@ -14007,7 +14054,7 @@
         <v>0021</v>
       </c>
       <c r="F6" s="266" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
@@ -14023,7 +14070,7 @@
         <v>0022</v>
       </c>
       <c r="F7" s="266" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -14039,7 +14086,7 @@
         <v>0023</v>
       </c>
       <c r="F8" s="266" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
@@ -14055,7 +14102,7 @@
         <v>0024</v>
       </c>
       <c r="F9" s="266" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -14071,7 +14118,7 @@
         <v>0025</v>
       </c>
       <c r="F10" s="266" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -14087,7 +14134,7 @@
         <v>0026</v>
       </c>
       <c r="F11" s="266" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -14103,7 +14150,7 @@
         <v>0027</v>
       </c>
       <c r="F12" s="266" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
@@ -14138,7 +14185,7 @@
         <v>159</v>
       </c>
       <c r="C15" s="218" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D15" s="218">
         <v>1</v>
@@ -14194,7 +14241,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>1</v>
       </c>
@@ -14203,7 +14250,7 @@
         <v>1010</v>
       </c>
       <c r="F17" s="266" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G17" s="34">
         <v>4</v>
@@ -14232,7 +14279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>2</v>
       </c>
@@ -14241,7 +14288,7 @@
         <v>1020</v>
       </c>
       <c r="F18" s="266" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G18" s="34">
         <v>4</v>
@@ -14263,10 +14310,10 @@
         <v>0</v>
       </c>
       <c r="N18" s="267" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>3</v>
       </c>
@@ -14275,7 +14322,7 @@
         <v>1030</v>
       </c>
       <c r="F19" s="266" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G19" s="34">
         <v>4</v>
@@ -14298,11 +14345,11 @@
         <v>0</v>
       </c>
       <c r="N19" s="267" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O19" s="264"/>
     </row>
-    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>4</v>
       </c>
@@ -14311,7 +14358,7 @@
         <v>1040</v>
       </c>
       <c r="F20" s="266" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G20" s="34">
         <v>4</v>
@@ -14337,7 +14384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>5</v>
       </c>
@@ -14346,7 +14393,7 @@
         <v>1050</v>
       </c>
       <c r="F21" s="266" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G21" s="34">
         <v>4</v>
@@ -14372,7 +14419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>6</v>
       </c>
@@ -14381,7 +14428,7 @@
         <v>1060</v>
       </c>
       <c r="F22" s="266" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G22" s="34">
         <v>4</v>
@@ -14407,7 +14454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>7</v>
       </c>
@@ -14416,7 +14463,7 @@
         <v>1070</v>
       </c>
       <c r="F23" s="266" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G23" s="34">
         <v>4</v>
@@ -14442,7 +14489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>8</v>
       </c>
@@ -14451,7 +14498,7 @@
         <v>1080</v>
       </c>
       <c r="F24" s="266" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G24" s="34">
         <v>4</v>
@@ -14477,7 +14524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>9</v>
       </c>
@@ -14486,7 +14533,7 @@
         <v>1090</v>
       </c>
       <c r="F25" s="266" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G25" s="34">
         <v>4</v>
@@ -14512,7 +14559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>10</v>
       </c>
@@ -14521,7 +14568,7 @@
         <v>10A0</v>
       </c>
       <c r="F26" s="266" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G26" s="34">
         <v>4</v>
@@ -14547,7 +14594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>11</v>
       </c>
@@ -14556,7 +14603,7 @@
         <v>10B0</v>
       </c>
       <c r="F27" s="266" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G27" s="34">
         <v>4</v>
@@ -14582,7 +14629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>12</v>
       </c>
@@ -14591,7 +14638,7 @@
         <v>10C0</v>
       </c>
       <c r="F28" s="266" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G28" s="34">
         <v>4</v>
@@ -14616,23 +14663,8 @@
       <c r="N28" s="65">
         <v>0</v>
       </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>100</v>
-      </c>
-      <c r="T28">
-        <v>35</v>
-      </c>
-      <c r="U28" t="s">
-        <v>246</v>
-      </c>
-      <c r="V28" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>13</v>
       </c>
@@ -14641,7 +14673,7 @@
         <v>10D0</v>
       </c>
       <c r="F29" s="266" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G29" s="34">
         <v>4</v>
@@ -14667,7 +14699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>14</v>
       </c>
@@ -14676,7 +14708,7 @@
         <v>10E0</v>
       </c>
       <c r="F30" s="266" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G30" s="34">
         <v>4</v>
@@ -14702,7 +14734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>15</v>
       </c>
@@ -14711,7 +14743,7 @@
         <v>10F0</v>
       </c>
       <c r="F31" s="266" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G31" s="34">
         <v>1</v>
@@ -14737,7 +14769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>16</v>
       </c>
@@ -14746,7 +14778,7 @@
         <v>1100</v>
       </c>
       <c r="F32" s="266" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G32" s="34">
         <v>1</v>
@@ -14781,7 +14813,7 @@
         <v>1110</v>
       </c>
       <c r="F33" s="266" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G33" s="34">
         <v>2</v>
@@ -14840,6 +14872,18 @@
       </c>
       <c r="N34" s="65">
         <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>100</v>
+      </c>
+      <c r="S34">
+        <v>35</v>
+      </c>
+      <c r="U34" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -14881,10 +14925,10 @@
     </row>
     <row r="38" spans="1:21" s="218" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="217" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C38" s="218" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D38" s="218">
         <v>2</v>
@@ -14911,7 +14955,7 @@
         <v>2000</v>
       </c>
       <c r="F39" s="266" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G39" s="34">
         <v>4</v>
@@ -14937,16 +14981,16 @@
         <v>1</v>
       </c>
       <c r="R39" t="s">
+        <v>277</v>
+      </c>
+      <c r="S39" t="s">
         <v>278</v>
-      </c>
-      <c r="S39" t="s">
-        <v>279</v>
       </c>
       <c r="T39">
         <v>10</v>
       </c>
       <c r="U39" t="s">
-        <v>176</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -14958,7 +15002,7 @@
         <v>2010</v>
       </c>
       <c r="F40" s="266" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G40" s="34">
         <v>4</v>
@@ -14984,13 +15028,19 @@
         <v>1</v>
       </c>
       <c r="P40" s="274" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R40" t="s">
+        <v>277</v>
+      </c>
+      <c r="S40" t="s">
         <v>278</v>
       </c>
-      <c r="S40" t="s">
-        <v>279</v>
+      <c r="T40" t="s">
+        <v>354</v>
+      </c>
+      <c r="U40" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -15002,7 +15052,7 @@
         <v>2020</v>
       </c>
       <c r="F41" s="266" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G41" s="34">
         <v>4</v>
@@ -15027,10 +15077,16 @@
         <v>1</v>
       </c>
       <c r="R41" t="s">
+        <v>277</v>
+      </c>
+      <c r="S41" t="s">
         <v>278</v>
       </c>
-      <c r="S41" t="s">
-        <v>279</v>
+      <c r="T41" t="s">
+        <v>355</v>
+      </c>
+      <c r="U41" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -15042,7 +15098,7 @@
         <v>2030</v>
       </c>
       <c r="F42" s="266" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G42" s="34">
         <v>4</v>
@@ -15076,7 +15132,7 @@
         <v>2040</v>
       </c>
       <c r="F43" s="266" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G43" s="34">
         <v>4</v>
@@ -15123,13 +15179,13 @@
     </row>
     <row r="46" spans="1:21" s="218" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="217" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B46" s="218" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C46" s="218" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D46" s="218">
         <v>3</v>
@@ -15156,7 +15212,7 @@
         <v>3000</v>
       </c>
       <c r="F47" s="266" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G47" s="34">
         <v>1</v>
@@ -15182,16 +15238,16 @@
         <v>1</v>
       </c>
       <c r="R47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="S47" t="s">
+        <v>308</v>
+      </c>
+      <c r="T47" t="s">
         <v>309</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
         <v>310</v>
-      </c>
-      <c r="U47" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -15203,7 +15259,7 @@
         <v>3010</v>
       </c>
       <c r="F48" s="266" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G48" s="34">
         <v>1</v>
@@ -15228,16 +15284,16 @@
         <v>1</v>
       </c>
       <c r="R48" t="s">
+        <v>311</v>
+      </c>
+      <c r="S48" t="s">
         <v>312</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
+        <v>314</v>
+      </c>
+      <c r="U48" t="s">
         <v>313</v>
-      </c>
-      <c r="T48" t="s">
-        <v>315</v>
-      </c>
-      <c r="U48" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -15249,7 +15305,7 @@
         <v>3020</v>
       </c>
       <c r="F49" s="266" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G49" s="34">
         <v>4</v>
@@ -15277,7 +15333,7 @@
         <v>0</v>
       </c>
       <c r="S49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -15289,7 +15345,7 @@
         <v>3030</v>
       </c>
       <c r="F50" s="266" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G50" s="34">
         <v>1</v>
@@ -15326,7 +15382,7 @@
         <v>3040</v>
       </c>
       <c r="F51" s="266" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G51" s="34">
         <v>1</v>
@@ -15363,7 +15419,7 @@
         <v>3050</v>
       </c>
       <c r="F52" s="266" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G52" s="34">
         <v>4</v>
@@ -15400,7 +15456,7 @@
         <v>3060</v>
       </c>
       <c r="F53" s="266" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G53" s="34">
         <v>1</v>
@@ -15437,7 +15493,7 @@
         <v>3070</v>
       </c>
       <c r="F54" s="266" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G54" s="34">
         <v>1</v>
@@ -15474,7 +15530,7 @@
         <v>3080</v>
       </c>
       <c r="F55" s="266" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G55" s="34">
         <v>4</v>
@@ -15511,7 +15567,7 @@
         <v>3090</v>
       </c>
       <c r="F56" s="266" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G56" s="34">
         <v>1</v>
@@ -15548,7 +15604,7 @@
         <v>30A0</v>
       </c>
       <c r="F57" s="266" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G57" s="34">
         <v>1</v>
@@ -15585,7 +15641,7 @@
         <v>30B0</v>
       </c>
       <c r="F58" s="266" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G58" s="34">
         <v>4</v>
@@ -15622,7 +15678,7 @@
         <v>30C0</v>
       </c>
       <c r="F59" s="266" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G59" s="34">
         <v>1</v>
@@ -15659,7 +15715,7 @@
         <v>30D0</v>
       </c>
       <c r="F60" s="266" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G60" s="34">
         <v>1</v>
@@ -15696,7 +15752,7 @@
         <v>30E0</v>
       </c>
       <c r="F61" s="266" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G61" s="34">
         <v>4</v>
@@ -15729,13 +15785,13 @@
     </row>
     <row r="63" spans="1:19" s="218" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="218" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B63" s="218" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C63" s="218" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D63" s="218">
         <v>4</v>

</xml_diff>